<commit_message>
Implemented new loss function for network models
</commit_message>
<xml_diff>
--- a/Brent3COVIDMetrics/rollingTestMetrics.xlsx
+++ b/Brent3COVIDMetrics/rollingTestMetrics.xlsx
@@ -497,22 +497,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.21</v>
+        <v>0.169</v>
       </c>
       <c r="C3" t="n">
-        <v>1.395</v>
+        <v>1.416</v>
       </c>
       <c r="D3" t="n">
-        <v>5.453</v>
+        <v>5.737</v>
       </c>
       <c r="E3" t="n">
-        <v>2.335</v>
+        <v>2.395</v>
       </c>
       <c r="F3" t="n">
-        <v>2.263</v>
+        <v>2.26</v>
       </c>
       <c r="G3" t="n">
-        <v>0.74</v>
+        <v>0.8070000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -522,22 +522,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.02</v>
+        <v>0.453</v>
       </c>
       <c r="C4" t="n">
-        <v>1.51</v>
+        <v>1.273</v>
       </c>
       <c r="D4" t="n">
-        <v>7.037</v>
+        <v>3.776</v>
       </c>
       <c r="E4" t="n">
-        <v>2.653</v>
+        <v>1.943</v>
       </c>
       <c r="F4" t="n">
-        <v>2.6</v>
+        <v>2.674</v>
       </c>
       <c r="G4" t="n">
-        <v>0.442</v>
+        <v>0.698</v>
       </c>
     </row>
     <row r="5">
@@ -547,22 +547,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.333</v>
+        <v>0.139</v>
       </c>
       <c r="C5" t="n">
-        <v>4.999</v>
+        <v>3.583</v>
       </c>
       <c r="D5" t="n">
-        <v>9.196999999999999</v>
+        <v>5.943</v>
       </c>
       <c r="E5" t="n">
-        <v>3.033</v>
+        <v>2.438</v>
       </c>
       <c r="F5" t="n">
-        <v>2.41</v>
+        <v>2.291</v>
       </c>
       <c r="G5" t="n">
-        <v>0.211</v>
+        <v>0.5629999999999999</v>
       </c>
     </row>
     <row r="6">
@@ -572,22 +572,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.218</v>
+        <v>0.211</v>
       </c>
       <c r="C6" t="n">
-        <v>1.391</v>
+        <v>1.394</v>
       </c>
       <c r="D6" t="n">
-        <v>5.397</v>
+        <v>5.446</v>
       </c>
       <c r="E6" t="n">
-        <v>2.323</v>
+        <v>2.334</v>
       </c>
       <c r="F6" t="n">
         <v>2.285</v>
       </c>
       <c r="G6" t="n">
-        <v>0.745</v>
+        <v>0.764</v>
       </c>
     </row>
     <row r="7">
@@ -622,22 +622,22 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.163</v>
+        <v>-0.112</v>
       </c>
       <c r="C8" t="n">
-        <v>1.582</v>
+        <v>1.556</v>
       </c>
       <c r="D8" t="n">
-        <v>0.739</v>
+        <v>0.706</v>
       </c>
       <c r="E8" t="n">
-        <v>0.86</v>
+        <v>0.84</v>
       </c>
       <c r="F8" t="n">
-        <v>0.704</v>
+        <v>0.681</v>
       </c>
       <c r="G8" t="n">
-        <v>0.154</v>
+        <v>0.155</v>
       </c>
     </row>
     <row r="9">
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.059</v>
+        <v>0.021</v>
       </c>
       <c r="C9" t="n">
-        <v>1.53</v>
+        <v>1.49</v>
       </c>
       <c r="D9" t="n">
-        <v>0.673</v>
+        <v>0.622</v>
       </c>
       <c r="E9" t="n">
-        <v>0.82</v>
+        <v>0.789</v>
       </c>
       <c r="F9" t="n">
-        <v>0.6919999999999999</v>
+        <v>0.664</v>
       </c>
       <c r="G9" t="n">
-        <v>0.311</v>
+        <v>0.278</v>
       </c>
     </row>
     <row r="10">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-1.441</v>
+        <v>-0.925</v>
       </c>
       <c r="C10" t="n">
-        <v>8.323</v>
+        <v>6.775</v>
       </c>
       <c r="D10" t="n">
-        <v>1.55</v>
+        <v>1.223</v>
       </c>
       <c r="E10" t="n">
-        <v>1.245</v>
+        <v>1.106</v>
       </c>
       <c r="F10" t="n">
-        <v>0.891</v>
+        <v>0.882</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.08699999999999999</v>
+        <v>0.104</v>
       </c>
     </row>
     <row r="11">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.198</v>
+        <v>-0.066</v>
       </c>
       <c r="C11" t="n">
-        <v>1.599</v>
+        <v>1.533</v>
       </c>
       <c r="D11" t="n">
-        <v>0.761</v>
+        <v>0.677</v>
       </c>
       <c r="E11" t="n">
-        <v>0.872</v>
+        <v>0.823</v>
       </c>
       <c r="F11" t="n">
-        <v>0.666</v>
+        <v>0.707</v>
       </c>
       <c r="G11" t="n">
-        <v>0.043</v>
+        <v>0.227</v>
       </c>
     </row>
     <row r="12">
@@ -747,10 +747,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-1.177</v>
+        <v>-1.178</v>
       </c>
       <c r="C13" t="n">
-        <v>2.088</v>
+        <v>2.089</v>
       </c>
       <c r="D13" t="n">
         <v>0.38</v>
@@ -759,10 +759,10 @@
         <v>0.616</v>
       </c>
       <c r="F13" t="n">
-        <v>0.524</v>
+        <v>0.521</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.004</v>
+        <v>-0.049</v>
       </c>
     </row>
     <row r="14">
@@ -772,22 +772,22 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.931</v>
+        <v>-2.074</v>
       </c>
       <c r="C14" t="n">
-        <v>1.966</v>
+        <v>2.537</v>
       </c>
       <c r="D14" t="n">
-        <v>0.337</v>
+        <v>0.536</v>
       </c>
       <c r="E14" t="n">
-        <v>0.581</v>
+        <v>0.732</v>
       </c>
       <c r="F14" t="n">
-        <v>0.5580000000000001</v>
+        <v>0.629</v>
       </c>
       <c r="G14" t="n">
-        <v>0.311</v>
+        <v>0.204</v>
       </c>
     </row>
     <row r="15">
@@ -797,22 +797,22 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.868</v>
+        <v>-1.181</v>
       </c>
       <c r="C15" t="n">
-        <v>6.604</v>
+        <v>7.543</v>
       </c>
       <c r="D15" t="n">
-        <v>0.326</v>
+        <v>0.381</v>
       </c>
       <c r="E15" t="n">
-        <v>0.571</v>
+        <v>0.617</v>
       </c>
       <c r="F15" t="n">
-        <v>0.46</v>
+        <v>0.551</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.452</v>
+        <v>0.047</v>
       </c>
     </row>
     <row r="16">
@@ -822,22 +822,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-1.201</v>
+        <v>-1.176</v>
       </c>
       <c r="C16" t="n">
-        <v>2.101</v>
+        <v>2.088</v>
       </c>
       <c r="D16" t="n">
-        <v>0.384</v>
+        <v>0.38</v>
       </c>
       <c r="E16" t="n">
-        <v>0.62</v>
+        <v>0.616</v>
       </c>
       <c r="F16" t="n">
-        <v>0.488</v>
+        <v>0.453</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.045</v>
+        <v>-0.183</v>
       </c>
     </row>
     <row r="17">
@@ -872,22 +872,22 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.305</v>
+        <v>0.187</v>
       </c>
       <c r="C18" t="n">
-        <v>1.348</v>
+        <v>1.406</v>
       </c>
       <c r="D18" t="n">
-        <v>0.546</v>
+        <v>0.639</v>
       </c>
       <c r="E18" t="n">
-        <v>0.739</v>
+        <v>0.799</v>
       </c>
       <c r="F18" t="n">
-        <v>0.892</v>
+        <v>0.911</v>
       </c>
       <c r="G18" t="n">
-        <v>0.747</v>
+        <v>0.643</v>
       </c>
     </row>
     <row r="19">
@@ -897,22 +897,22 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.169</v>
+        <v>0.279</v>
       </c>
       <c r="C19" t="n">
-        <v>1.416</v>
+        <v>1.36</v>
       </c>
       <c r="D19" t="n">
-        <v>0.653</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="E19" t="n">
-        <v>0.8080000000000001</v>
+        <v>0.753</v>
       </c>
       <c r="F19" t="n">
-        <v>0.866</v>
+        <v>0.801</v>
       </c>
       <c r="G19" t="n">
-        <v>0.538</v>
+        <v>0.5629999999999999</v>
       </c>
     </row>
     <row r="20">
@@ -922,22 +922,22 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.037</v>
+        <v>0.406</v>
       </c>
       <c r="C20" t="n">
-        <v>4.111</v>
+        <v>2.782</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8149999999999999</v>
+        <v>0.467</v>
       </c>
       <c r="E20" t="n">
-        <v>0.903</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="F20" t="n">
-        <v>0.8090000000000001</v>
+        <v>0.8080000000000001</v>
       </c>
       <c r="G20" t="n">
-        <v>0.517</v>
+        <v>0.716</v>
       </c>
     </row>
     <row r="21">
@@ -947,22 +947,22 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.134</v>
+        <v>0.209</v>
       </c>
       <c r="C21" t="n">
-        <v>1.433</v>
+        <v>1.396</v>
       </c>
       <c r="D21" t="n">
-        <v>0.68</v>
+        <v>0.622</v>
       </c>
       <c r="E21" t="n">
-        <v>0.825</v>
+        <v>0.789</v>
       </c>
       <c r="F21" t="n">
-        <v>0.854</v>
+        <v>0.833</v>
       </c>
       <c r="G21" t="n">
-        <v>0.6820000000000001</v>
+        <v>0.627</v>
       </c>
     </row>
     <row r="22">
@@ -997,22 +997,22 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.246</v>
+        <v>0.23</v>
       </c>
       <c r="C23" t="n">
-        <v>1.377</v>
+        <v>1.385</v>
       </c>
       <c r="D23" t="n">
-        <v>0.669</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="E23" t="n">
-        <v>0.8179999999999999</v>
+        <v>0.826</v>
       </c>
       <c r="F23" t="n">
         <v>0.946</v>
       </c>
       <c r="G23" t="n">
-        <v>0.665</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="24">
@@ -1022,22 +1022,22 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.349</v>
+        <v>0.162</v>
       </c>
       <c r="C24" t="n">
-        <v>1.326</v>
+        <v>1.419</v>
       </c>
       <c r="D24" t="n">
-        <v>0.577</v>
+        <v>0.743</v>
       </c>
       <c r="E24" t="n">
-        <v>0.76</v>
+        <v>0.862</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9360000000000001</v>
+        <v>0.97</v>
       </c>
       <c r="G24" t="n">
-        <v>0.658</v>
+        <v>0.507</v>
       </c>
     </row>
     <row r="25">
@@ -1047,22 +1047,22 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.102</v>
+        <v>0.239</v>
       </c>
       <c r="C25" t="n">
-        <v>3.694</v>
+        <v>3.283</v>
       </c>
       <c r="D25" t="n">
-        <v>0.796</v>
+        <v>0.675</v>
       </c>
       <c r="E25" t="n">
-        <v>0.892</v>
+        <v>0.822</v>
       </c>
       <c r="F25" t="n">
-        <v>0.983</v>
+        <v>1.014</v>
       </c>
       <c r="G25" t="n">
-        <v>0.662</v>
+        <v>0.643</v>
       </c>
     </row>
     <row r="26">
@@ -1072,22 +1072,22 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.291</v>
+        <v>0.295</v>
       </c>
       <c r="C26" t="n">
-        <v>1.354</v>
+        <v>1.352</v>
       </c>
       <c r="D26" t="n">
-        <v>0.628</v>
+        <v>0.625</v>
       </c>
       <c r="E26" t="n">
-        <v>0.792</v>
+        <v>0.791</v>
       </c>
       <c r="F26" t="n">
-        <v>0.923</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="G26" t="n">
-        <v>0.579</v>
+        <v>0.619</v>
       </c>
     </row>
     <row r="27">
@@ -1122,22 +1122,22 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.315</v>
+        <v>0.242</v>
       </c>
       <c r="C28" t="n">
-        <v>1.342</v>
+        <v>1.379</v>
       </c>
       <c r="D28" t="n">
-        <v>0.858</v>
+        <v>0.95</v>
       </c>
       <c r="E28" t="n">
-        <v>0.926</v>
+        <v>0.975</v>
       </c>
       <c r="F28" t="n">
-        <v>1.046</v>
+        <v>1.048</v>
       </c>
       <c r="G28" t="n">
-        <v>0.633</v>
+        <v>0.569</v>
       </c>
     </row>
     <row r="29">
@@ -1147,22 +1147,22 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.363</v>
+        <v>0.34</v>
       </c>
       <c r="C29" t="n">
-        <v>1.318</v>
+        <v>1.33</v>
       </c>
       <c r="D29" t="n">
-        <v>0.798</v>
+        <v>0.827</v>
       </c>
       <c r="E29" t="n">
-        <v>0.893</v>
+        <v>0.909</v>
       </c>
       <c r="F29" t="n">
-        <v>1.053</v>
+        <v>1.031</v>
       </c>
       <c r="G29" t="n">
-        <v>0.628</v>
+        <v>0.604</v>
       </c>
     </row>
     <row r="30">
@@ -1172,22 +1172,22 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.288</v>
+        <v>0.1</v>
       </c>
       <c r="C30" t="n">
-        <v>3.136</v>
+        <v>3.7</v>
       </c>
       <c r="D30" t="n">
-        <v>0.892</v>
+        <v>1.127</v>
       </c>
       <c r="E30" t="n">
-        <v>0.944</v>
+        <v>1.062</v>
       </c>
       <c r="F30" t="n">
-        <v>1.041</v>
+        <v>1.106</v>
       </c>
       <c r="G30" t="n">
-        <v>0.664</v>
+        <v>0.547</v>
       </c>
     </row>
     <row r="31">
@@ -1197,22 +1197,22 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.329</v>
+        <v>0.313</v>
       </c>
       <c r="C31" t="n">
-        <v>1.336</v>
+        <v>1.344</v>
       </c>
       <c r="D31" t="n">
-        <v>0.841</v>
+        <v>0.861</v>
       </c>
       <c r="E31" t="n">
-        <v>0.917</v>
+        <v>0.928</v>
       </c>
       <c r="F31" t="n">
-        <v>1.043</v>
+        <v>1.033</v>
       </c>
       <c r="G31" t="n">
-        <v>0.592</v>
+        <v>0.586</v>
       </c>
     </row>
     <row r="32">
@@ -1247,22 +1247,22 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.043</v>
+        <v>0.143</v>
       </c>
       <c r="C33" t="n">
-        <v>1.478</v>
+        <v>1.428</v>
       </c>
       <c r="D33" t="n">
-        <v>0.328</v>
+        <v>0.294</v>
       </c>
       <c r="E33" t="n">
-        <v>0.573</v>
+        <v>0.542</v>
       </c>
       <c r="F33" t="n">
-        <v>0.571</v>
+        <v>0.592</v>
       </c>
       <c r="G33" t="n">
-        <v>0.455</v>
+        <v>0.577</v>
       </c>
     </row>
     <row r="34">
@@ -1272,22 +1272,22 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-0.059</v>
+        <v>0.063</v>
       </c>
       <c r="C34" t="n">
-        <v>1.53</v>
+        <v>1.468</v>
       </c>
       <c r="D34" t="n">
-        <v>0.363</v>
+        <v>0.321</v>
       </c>
       <c r="E34" t="n">
-        <v>0.602</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="F34" t="n">
-        <v>0.647</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="G34" t="n">
-        <v>0.575</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="35">
@@ -1297,22 +1297,22 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.35</v>
+        <v>-0.062</v>
       </c>
       <c r="C35" t="n">
-        <v>2.95</v>
+        <v>4.186</v>
       </c>
       <c r="D35" t="n">
-        <v>0.223</v>
+        <v>0.364</v>
       </c>
       <c r="E35" t="n">
-        <v>0.472</v>
+        <v>0.603</v>
       </c>
       <c r="F35" t="n">
-        <v>0.622</v>
+        <v>0.665</v>
       </c>
       <c r="G35" t="n">
-        <v>0.716</v>
+        <v>0.596</v>
       </c>
     </row>
     <row r="36">
@@ -1322,22 +1322,22 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.217</v>
+        <v>0.191</v>
       </c>
       <c r="C36" t="n">
-        <v>1.392</v>
+        <v>1.404</v>
       </c>
       <c r="D36" t="n">
-        <v>0.268</v>
+        <v>0.277</v>
       </c>
       <c r="E36" t="n">
-        <v>0.518</v>
+        <v>0.526</v>
       </c>
       <c r="F36" t="n">
-        <v>0.543</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="G36" t="n">
-        <v>0.5639999999999999</v>
+        <v>0.516</v>
       </c>
     </row>
     <row r="37">
@@ -1372,22 +1372,22 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.204</v>
+        <v>0.248</v>
       </c>
       <c r="C38" t="n">
-        <v>1.398</v>
+        <v>1.376</v>
       </c>
       <c r="D38" t="n">
-        <v>0.929</v>
+        <v>0.878</v>
       </c>
       <c r="E38" t="n">
-        <v>0.964</v>
+        <v>0.9370000000000001</v>
       </c>
       <c r="F38" t="n">
-        <v>0.974</v>
+        <v>0.972</v>
       </c>
       <c r="G38" t="n">
-        <v>0.6850000000000001</v>
+        <v>0.744</v>
       </c>
     </row>
     <row r="39">
@@ -1397,22 +1397,22 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.571</v>
+        <v>0.415</v>
       </c>
       <c r="C39" t="n">
-        <v>1.215</v>
+        <v>1.292</v>
       </c>
       <c r="D39" t="n">
-        <v>0.501</v>
+        <v>0.6820000000000001</v>
       </c>
       <c r="E39" t="n">
-        <v>0.708</v>
+        <v>0.826</v>
       </c>
       <c r="F39" t="n">
-        <v>0.982</v>
+        <v>0.952</v>
       </c>
       <c r="G39" t="n">
-        <v>0.864</v>
+        <v>0.852</v>
       </c>
     </row>
     <row r="40">
@@ -1422,22 +1422,22 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.278</v>
+        <v>0.205</v>
       </c>
       <c r="C40" t="n">
-        <v>3.166</v>
+        <v>3.385</v>
       </c>
       <c r="D40" t="n">
-        <v>0.841</v>
+        <v>0.927</v>
       </c>
       <c r="E40" t="n">
-        <v>0.917</v>
+        <v>0.963</v>
       </c>
       <c r="F40" t="n">
-        <v>0.953</v>
+        <v>0.999</v>
       </c>
       <c r="G40" t="n">
-        <v>0.865</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="41">
@@ -1447,22 +1447,22 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.247</v>
+        <v>0.276</v>
       </c>
       <c r="C41" t="n">
-        <v>1.376</v>
+        <v>1.362</v>
       </c>
       <c r="D41" t="n">
-        <v>0.879</v>
+        <v>0.845</v>
       </c>
       <c r="E41" t="n">
-        <v>0.9379999999999999</v>
+        <v>0.919</v>
       </c>
       <c r="F41" t="n">
-        <v>0.961</v>
+        <v>0.97</v>
       </c>
       <c r="G41" t="n">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="42">
@@ -1497,22 +1497,22 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.481</v>
+        <v>0.469</v>
       </c>
       <c r="C43" t="n">
-        <v>1.26</v>
+        <v>1.266</v>
       </c>
       <c r="D43" t="n">
-        <v>0.465</v>
+        <v>0.476</v>
       </c>
       <c r="E43" t="n">
-        <v>0.6820000000000001</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F43" t="n">
-        <v>0.913</v>
+        <v>0.904</v>
       </c>
       <c r="G43" t="n">
-        <v>0.722</v>
+        <v>0.756</v>
       </c>
     </row>
     <row r="44">
@@ -1522,22 +1522,22 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>-0.004</v>
+        <v>0.264</v>
       </c>
       <c r="C44" t="n">
-        <v>1.502</v>
+        <v>1.368</v>
       </c>
       <c r="D44" t="n">
-        <v>0.899</v>
+        <v>0.659</v>
       </c>
       <c r="E44" t="n">
-        <v>0.948</v>
+        <v>0.8120000000000001</v>
       </c>
       <c r="F44" t="n">
-        <v>1.116</v>
+        <v>0.856</v>
       </c>
       <c r="G44" t="n">
-        <v>0.547</v>
+        <v>0.595</v>
       </c>
     </row>
     <row r="45">
@@ -1547,22 +1547,22 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.14</v>
+        <v>0.045</v>
       </c>
       <c r="C45" t="n">
-        <v>3.58</v>
+        <v>3.865</v>
       </c>
       <c r="D45" t="n">
-        <v>0.77</v>
+        <v>0.856</v>
       </c>
       <c r="E45" t="n">
-        <v>0.877</v>
+        <v>0.925</v>
       </c>
       <c r="F45" t="n">
-        <v>0.858</v>
+        <v>0.852</v>
       </c>
       <c r="G45" t="n">
-        <v>0.375</v>
+        <v>0.229</v>
       </c>
     </row>
     <row r="46">
@@ -1572,22 +1572,22 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.503</v>
+        <v>0.543</v>
       </c>
       <c r="C46" t="n">
-        <v>1.248</v>
+        <v>1.228</v>
       </c>
       <c r="D46" t="n">
-        <v>0.445</v>
+        <v>0.41</v>
       </c>
       <c r="E46" t="n">
-        <v>0.667</v>
+        <v>0.64</v>
       </c>
       <c r="F46" t="n">
-        <v>0.888</v>
+        <v>0.88</v>
       </c>
       <c r="G46" t="n">
-        <v>0.749</v>
+        <v>0.8070000000000001</v>
       </c>
     </row>
     <row r="47">
@@ -1622,22 +1622,22 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.242</v>
+        <v>0.227</v>
       </c>
       <c r="C48" t="n">
-        <v>1.379</v>
+        <v>1.386</v>
       </c>
       <c r="D48" t="n">
-        <v>0.478</v>
+        <v>0.488</v>
       </c>
       <c r="E48" t="n">
-        <v>0.6909999999999999</v>
+        <v>0.699</v>
       </c>
       <c r="F48" t="n">
-        <v>0.834</v>
+        <v>0.851</v>
       </c>
       <c r="G48" t="n">
-        <v>0.645</v>
+        <v>0.631</v>
       </c>
     </row>
     <row r="49">
@@ -1647,22 +1647,22 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.273</v>
+        <v>0.354</v>
       </c>
       <c r="C49" t="n">
-        <v>1.364</v>
+        <v>1.323</v>
       </c>
       <c r="D49" t="n">
-        <v>0.459</v>
+        <v>0.408</v>
       </c>
       <c r="E49" t="n">
-        <v>0.677</v>
+        <v>0.639</v>
       </c>
       <c r="F49" t="n">
-        <v>0.926</v>
+        <v>0.765</v>
       </c>
       <c r="G49" t="n">
-        <v>0.668</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="50">
@@ -1672,22 +1672,22 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.621</v>
+        <v>0.442</v>
       </c>
       <c r="C50" t="n">
-        <v>2.137</v>
+        <v>2.674</v>
       </c>
       <c r="D50" t="n">
-        <v>0.239</v>
+        <v>0.352</v>
       </c>
       <c r="E50" t="n">
-        <v>0.489</v>
+        <v>0.593</v>
       </c>
       <c r="F50" t="n">
-        <v>0.764</v>
+        <v>0.713</v>
       </c>
       <c r="G50" t="n">
-        <v>0.873</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="51">
@@ -1697,22 +1697,22 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.343</v>
+        <v>0.446</v>
       </c>
       <c r="C51" t="n">
-        <v>1.328</v>
+        <v>1.277</v>
       </c>
       <c r="D51" t="n">
-        <v>0.415</v>
+        <v>0.35</v>
       </c>
       <c r="E51" t="n">
-        <v>0.644</v>
+        <v>0.592</v>
       </c>
       <c r="F51" t="n">
-        <v>0.8120000000000001</v>
+        <v>0.792</v>
       </c>
       <c r="G51" t="n">
-        <v>0.662</v>
+        <v>0.707</v>
       </c>
     </row>
     <row r="52">
@@ -1747,22 +1747,22 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.184</v>
+        <v>0.186</v>
       </c>
       <c r="C53" t="n">
-        <v>1.408</v>
+        <v>1.407</v>
       </c>
       <c r="D53" t="n">
-        <v>0.247</v>
+        <v>0.246</v>
       </c>
       <c r="E53" t="n">
-        <v>0.497</v>
+        <v>0.496</v>
       </c>
       <c r="F53" t="n">
-        <v>0.536</v>
+        <v>0.551</v>
       </c>
       <c r="G53" t="n">
-        <v>0.493</v>
+        <v>0.511</v>
       </c>
     </row>
     <row r="54">
@@ -1772,22 +1772,22 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.435</v>
+        <v>0.537</v>
       </c>
       <c r="C54" t="n">
-        <v>1.282</v>
+        <v>1.232</v>
       </c>
       <c r="D54" t="n">
-        <v>0.171</v>
+        <v>0.14</v>
       </c>
       <c r="E54" t="n">
-        <v>0.414</v>
+        <v>0.374</v>
       </c>
       <c r="F54" t="n">
-        <v>0.536</v>
+        <v>0.569</v>
       </c>
       <c r="G54" t="n">
-        <v>0.6840000000000001</v>
+        <v>0.746</v>
       </c>
     </row>
     <row r="55">
@@ -1797,22 +1797,22 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.359</v>
+        <v>-0.641</v>
       </c>
       <c r="C55" t="n">
-        <v>2.923</v>
+        <v>5.923</v>
       </c>
       <c r="D55" t="n">
-        <v>0.194</v>
+        <v>0.496</v>
       </c>
       <c r="E55" t="n">
-        <v>0.44</v>
+        <v>0.704</v>
       </c>
       <c r="F55" t="n">
-        <v>0.512</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="G55" t="n">
-        <v>0.599</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="56">
@@ -1822,22 +1822,22 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.197</v>
+        <v>0.247</v>
       </c>
       <c r="C56" t="n">
-        <v>1.402</v>
+        <v>1.376</v>
       </c>
       <c r="D56" t="n">
-        <v>0.243</v>
+        <v>0.227</v>
       </c>
       <c r="E56" t="n">
-        <v>0.493</v>
+        <v>0.476</v>
       </c>
       <c r="F56" t="n">
-        <v>0.541</v>
+        <v>0.549</v>
       </c>
       <c r="G56" t="n">
-        <v>0.528</v>
+        <v>0.5629999999999999</v>
       </c>
     </row>
     <row r="57">
@@ -1872,22 +1872,22 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>-0.152</v>
+        <v>-0.181</v>
       </c>
       <c r="C58" t="n">
-        <v>1.576</v>
+        <v>1.59</v>
       </c>
       <c r="D58" t="n">
-        <v>0.5620000000000001</v>
+        <v>0.576</v>
       </c>
       <c r="E58" t="n">
-        <v>0.75</v>
+        <v>0.759</v>
       </c>
       <c r="F58" t="n">
-        <v>0.737</v>
+        <v>0.747</v>
       </c>
       <c r="G58" t="n">
-        <v>0.31</v>
+        <v>0.309</v>
       </c>
     </row>
     <row r="59">
@@ -1897,22 +1897,22 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>-0.14</v>
+        <v>0.043</v>
       </c>
       <c r="C59" t="n">
-        <v>1.57</v>
+        <v>1.478</v>
       </c>
       <c r="D59" t="n">
-        <v>0.556</v>
+        <v>0.467</v>
       </c>
       <c r="E59" t="n">
-        <v>0.746</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="F59" t="n">
-        <v>0.707</v>
+        <v>0.738</v>
       </c>
       <c r="G59" t="n">
-        <v>0.213</v>
+        <v>0.405</v>
       </c>
     </row>
     <row r="60">
@@ -1922,22 +1922,22 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.246</v>
+        <v>0.136</v>
       </c>
       <c r="C60" t="n">
-        <v>3.262</v>
+        <v>3.592</v>
       </c>
       <c r="D60" t="n">
-        <v>0.368</v>
+        <v>0.422</v>
       </c>
       <c r="E60" t="n">
-        <v>0.607</v>
+        <v>0.65</v>
       </c>
       <c r="F60" t="n">
-        <v>0.731</v>
+        <v>0.784</v>
       </c>
       <c r="G60" t="n">
-        <v>0.695</v>
+        <v>0.5629999999999999</v>
       </c>
     </row>
     <row r="61">
@@ -1947,22 +1947,22 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.07099999999999999</v>
+        <v>-0.074</v>
       </c>
       <c r="C61" t="n">
-        <v>1.465</v>
+        <v>1.537</v>
       </c>
       <c r="D61" t="n">
-        <v>0.453</v>
+        <v>0.524</v>
       </c>
       <c r="E61" t="n">
-        <v>0.673</v>
+        <v>0.724</v>
       </c>
       <c r="F61" t="n">
-        <v>0.68</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="G61" t="n">
-        <v>0.335</v>
+        <v>0.231</v>
       </c>
     </row>
     <row r="62">
@@ -1997,22 +1997,22 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.253</v>
+        <v>0.304</v>
       </c>
       <c r="C63" t="n">
-        <v>1.374</v>
+        <v>1.348</v>
       </c>
       <c r="D63" t="n">
-        <v>0.373</v>
+        <v>0.348</v>
       </c>
       <c r="E63" t="n">
-        <v>0.611</v>
+        <v>0.59</v>
       </c>
       <c r="F63" t="n">
-        <v>0.71</v>
+        <v>0.733</v>
       </c>
       <c r="G63" t="n">
-        <v>0.601</v>
+        <v>0.6919999999999999</v>
       </c>
     </row>
     <row r="64">
@@ -2022,22 +2022,22 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>-0.019</v>
+        <v>0.253</v>
       </c>
       <c r="C64" t="n">
-        <v>1.51</v>
+        <v>1.374</v>
       </c>
       <c r="D64" t="n">
-        <v>0.51</v>
+        <v>0.373</v>
       </c>
       <c r="E64" t="n">
-        <v>0.714</v>
+        <v>0.611</v>
       </c>
       <c r="F64" t="n">
-        <v>0.617</v>
+        <v>0.609</v>
       </c>
       <c r="G64" t="n">
-        <v>0.295</v>
+        <v>0.593</v>
       </c>
     </row>
     <row r="65">
@@ -2047,22 +2047,22 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.273</v>
+        <v>0.176</v>
       </c>
       <c r="C65" t="n">
-        <v>3.181</v>
+        <v>3.472</v>
       </c>
       <c r="D65" t="n">
-        <v>0.363</v>
+        <v>0.412</v>
       </c>
       <c r="E65" t="n">
-        <v>0.602</v>
+        <v>0.642</v>
       </c>
       <c r="F65" t="n">
-        <v>0.5639999999999999</v>
+        <v>0.59</v>
       </c>
       <c r="G65" t="n">
-        <v>0.729</v>
+        <v>0.441</v>
       </c>
     </row>
     <row r="66">
@@ -2072,22 +2072,22 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.37</v>
+        <v>0.286</v>
       </c>
       <c r="C66" t="n">
-        <v>1.315</v>
+        <v>1.357</v>
       </c>
       <c r="D66" t="n">
-        <v>0.315</v>
+        <v>0.357</v>
       </c>
       <c r="E66" t="n">
-        <v>0.5610000000000001</v>
+        <v>0.597</v>
       </c>
       <c r="F66" t="n">
-        <v>0.697</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="G66" t="n">
-        <v>0.658</v>
+        <v>0.601</v>
       </c>
     </row>
     <row r="67">
@@ -2122,22 +2122,22 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.702</v>
+        <v>0.661</v>
       </c>
       <c r="C68" t="n">
-        <v>1.149</v>
+        <v>1.17</v>
       </c>
       <c r="D68" t="n">
-        <v>0.117</v>
+        <v>0.134</v>
       </c>
       <c r="E68" t="n">
-        <v>0.342</v>
+        <v>0.366</v>
       </c>
       <c r="F68" t="n">
-        <v>0.64</v>
+        <v>0.654</v>
       </c>
       <c r="G68" t="n">
-        <v>0.851</v>
+        <v>0.821</v>
       </c>
     </row>
     <row r="69">
@@ -2147,22 +2147,22 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="C69" t="n">
-        <v>1.405</v>
+        <v>1.415</v>
       </c>
       <c r="D69" t="n">
-        <v>0.319</v>
+        <v>0.326</v>
       </c>
       <c r="E69" t="n">
-        <v>0.5649999999999999</v>
+        <v>0.571</v>
       </c>
       <c r="F69" t="n">
-        <v>0.6889999999999999</v>
+        <v>0.59</v>
       </c>
       <c r="G69" t="n">
-        <v>0.5639999999999999</v>
+        <v>0.461</v>
       </c>
     </row>
     <row r="70">
@@ -2172,22 +2172,22 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.546</v>
+        <v>0.514</v>
       </c>
       <c r="C70" t="n">
-        <v>2.362</v>
+        <v>2.458</v>
       </c>
       <c r="D70" t="n">
-        <v>0.178</v>
+        <v>0.191</v>
       </c>
       <c r="E70" t="n">
-        <v>0.422</v>
+        <v>0.437</v>
       </c>
       <c r="F70" t="n">
-        <v>0.573</v>
+        <v>0.578</v>
       </c>
       <c r="G70" t="n">
-        <v>0.78</v>
+        <v>0.753</v>
       </c>
     </row>
     <row r="71">
@@ -2197,22 +2197,22 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.617</v>
+        <v>0.65</v>
       </c>
       <c r="C71" t="n">
-        <v>1.192</v>
+        <v>1.175</v>
       </c>
       <c r="D71" t="n">
-        <v>0.151</v>
+        <v>0.138</v>
       </c>
       <c r="E71" t="n">
-        <v>0.389</v>
+        <v>0.371</v>
       </c>
       <c r="F71" t="n">
-        <v>0.594</v>
+        <v>0.595</v>
       </c>
       <c r="G71" t="n">
-        <v>0.805</v>
+        <v>0.837</v>
       </c>
     </row>
     <row r="72">
@@ -2247,22 +2247,22 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.102</v>
+        <v>0.036</v>
       </c>
       <c r="C73" t="n">
-        <v>1.449</v>
+        <v>1.482</v>
       </c>
       <c r="D73" t="n">
-        <v>0.918</v>
+        <v>0.985</v>
       </c>
       <c r="E73" t="n">
-        <v>0.958</v>
+        <v>0.992</v>
       </c>
       <c r="F73" t="n">
-        <v>0.993</v>
+        <v>0.981</v>
       </c>
       <c r="G73" t="n">
-        <v>0.475</v>
+        <v>0.423</v>
       </c>
     </row>
     <row r="74">
@@ -2272,22 +2272,22 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>-19.358</v>
+        <v>-1.969</v>
       </c>
       <c r="C74" t="n">
-        <v>11.179</v>
+        <v>2.484</v>
       </c>
       <c r="D74" t="n">
-        <v>20.819</v>
+        <v>3.036</v>
       </c>
       <c r="E74" t="n">
-        <v>4.563</v>
+        <v>1.742</v>
       </c>
       <c r="F74" t="n">
-        <v>2.417</v>
+        <v>1.207</v>
       </c>
       <c r="G74" t="n">
-        <v>-0.555</v>
+        <v>-0.318</v>
       </c>
     </row>
     <row r="75">
@@ -2297,22 +2297,22 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>-5.798</v>
+        <v>-12.306</v>
       </c>
       <c r="C75" t="n">
-        <v>21.394</v>
+        <v>40.918</v>
       </c>
       <c r="D75" t="n">
-        <v>6.952</v>
+        <v>13.608</v>
       </c>
       <c r="E75" t="n">
-        <v>2.637</v>
+        <v>3.689</v>
       </c>
       <c r="F75" t="n">
-        <v>1.691</v>
+        <v>1.944</v>
       </c>
       <c r="G75" t="n">
-        <v>-0.126</v>
+        <v>0.08400000000000001</v>
       </c>
     </row>
     <row r="76">
@@ -2322,22 +2322,22 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.221</v>
+        <v>0.538</v>
       </c>
       <c r="C76" t="n">
-        <v>1.39</v>
+        <v>1.231</v>
       </c>
       <c r="D76" t="n">
-        <v>0.797</v>
+        <v>0.473</v>
       </c>
       <c r="E76" t="n">
-        <v>0.893</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="F76" t="n">
-        <v>1.221</v>
+        <v>1.088</v>
       </c>
       <c r="G76" t="n">
-        <v>0.6889999999999999</v>
+        <v>0.772</v>
       </c>
     </row>
     <row r="77">
@@ -2372,19 +2372,19 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>-5.331</v>
+        <v>-4.759</v>
       </c>
       <c r="C78" t="n">
-        <v>1.244</v>
+        <v>1.222</v>
       </c>
       <c r="D78" t="n">
-        <v>2.699</v>
+        <v>2.455</v>
       </c>
       <c r="E78" t="n">
-        <v>1.643</v>
+        <v>1.567</v>
       </c>
       <c r="F78" t="n">
-        <v>1.642</v>
+        <v>1.563</v>
       </c>
       <c r="G78" t="n">
         <v>1</v>
@@ -2397,19 +2397,19 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>-214.693</v>
+        <v>-14.295</v>
       </c>
       <c r="C79" t="n">
-        <v>9.295999999999999</v>
+        <v>1.588</v>
       </c>
       <c r="D79" t="n">
-        <v>91.95999999999999</v>
+        <v>6.521</v>
       </c>
       <c r="E79" t="n">
-        <v>9.59</v>
+        <v>2.554</v>
       </c>
       <c r="F79" t="n">
-        <v>7.58</v>
+        <v>2.403</v>
       </c>
       <c r="G79" t="n">
         <v>-1</v>
@@ -2422,19 +2422,19 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>-9.124000000000001</v>
+        <v>-6.659</v>
       </c>
       <c r="C80" t="n">
-        <v>1.92</v>
+        <v>1.696</v>
       </c>
       <c r="D80" t="n">
-        <v>4.317</v>
+        <v>3.265</v>
       </c>
       <c r="E80" t="n">
-        <v>2.078</v>
+        <v>1.807</v>
       </c>
       <c r="F80" t="n">
-        <v>2.015</v>
+        <v>1.77</v>
       </c>
       <c r="G80" t="n">
         <v>1</v>
@@ -2447,19 +2447,19 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>-2015548.754</v>
+        <v>-2012651.233</v>
       </c>
       <c r="C81" t="n">
-        <v>77522.144</v>
+        <v>77410.701</v>
       </c>
       <c r="D81" t="n">
-        <v>859328.058</v>
+        <v>858092.702</v>
       </c>
       <c r="E81" t="n">
-        <v>926.999</v>
+        <v>926.333</v>
       </c>
       <c r="F81" t="n">
-        <v>673.758</v>
+        <v>673.208</v>
       </c>
       <c r="G81" t="n">
         <v>-1</v>
@@ -2497,19 +2497,19 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>-1.646</v>
+        <v>-1.848</v>
       </c>
       <c r="C83" t="n">
-        <v>1.102</v>
+        <v>1.11</v>
       </c>
       <c r="D83" t="n">
-        <v>1.648</v>
+        <v>1.775</v>
       </c>
       <c r="E83" t="n">
-        <v>1.284</v>
+        <v>1.332</v>
       </c>
       <c r="F83" t="n">
-        <v>1.604</v>
+        <v>1.655</v>
       </c>
       <c r="G83" t="n">
         <v>1</v>
@@ -2522,19 +2522,19 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>-4.806</v>
+        <v>-12.197</v>
       </c>
       <c r="C84" t="n">
-        <v>1.223</v>
+        <v>1.508</v>
       </c>
       <c r="D84" t="n">
-        <v>3.618</v>
+        <v>8.223000000000001</v>
       </c>
       <c r="E84" t="n">
-        <v>1.902</v>
+        <v>2.868</v>
       </c>
       <c r="F84" t="n">
-        <v>2.689</v>
+        <v>2.841</v>
       </c>
       <c r="G84" t="n">
         <v>1</v>
@@ -2547,19 +2547,19 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>-46.383</v>
+        <v>-114.507</v>
       </c>
       <c r="C85" t="n">
-        <v>5.308</v>
+        <v>11.501</v>
       </c>
       <c r="D85" t="n">
-        <v>29.521</v>
+        <v>71.96599999999999</v>
       </c>
       <c r="E85" t="n">
-        <v>5.433</v>
+        <v>8.483000000000001</v>
       </c>
       <c r="F85" t="n">
-        <v>5.234</v>
+        <v>7.199</v>
       </c>
       <c r="G85" t="n">
         <v>1</v>
@@ -2572,19 +2572,19 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>-1701322.093</v>
+        <v>-1699263.789</v>
       </c>
       <c r="C86" t="n">
-        <v>65436.504</v>
+        <v>65357.338</v>
       </c>
       <c r="D86" t="n">
-        <v>1059993.551</v>
+        <v>1058711.144</v>
       </c>
       <c r="E86" t="n">
-        <v>1029.56</v>
+        <v>1028.937</v>
       </c>
       <c r="F86" t="n">
-        <v>909.5119999999999</v>
+        <v>909.255</v>
       </c>
       <c r="G86" t="n">
         <v>-1</v>
@@ -2622,16 +2622,16 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>-0.874</v>
+        <v>-0.696</v>
       </c>
       <c r="C88" t="n">
-        <v>1.072</v>
+        <v>1.065</v>
       </c>
       <c r="D88" t="n">
-        <v>0.143</v>
+        <v>0.129</v>
       </c>
       <c r="E88" t="n">
-        <v>0.378</v>
+        <v>0.359</v>
       </c>
       <c r="F88" t="n">
         <v>0.276</v>
@@ -2647,19 +2647,19 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>-0.9379999999999999</v>
+        <v>-17.786</v>
       </c>
       <c r="C89" t="n">
-        <v>1.075</v>
+        <v>1.723</v>
       </c>
       <c r="D89" t="n">
-        <v>0.147</v>
+        <v>1.429</v>
       </c>
       <c r="E89" t="n">
-        <v>0.383</v>
+        <v>1.195</v>
       </c>
       <c r="F89" t="n">
-        <v>0.66</v>
+        <v>1.186</v>
       </c>
       <c r="G89" t="n">
         <v>1</v>
@@ -2672,22 +2672,22 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>-41.667</v>
+        <v>-2.723</v>
       </c>
       <c r="C90" t="n">
-        <v>4.879</v>
+        <v>1.338</v>
       </c>
       <c r="D90" t="n">
-        <v>3.245</v>
+        <v>0.283</v>
       </c>
       <c r="E90" t="n">
-        <v>1.801</v>
+        <v>0.532</v>
       </c>
       <c r="F90" t="n">
-        <v>1.26</v>
+        <v>0.649</v>
       </c>
       <c r="G90" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
@@ -2697,22 +2697,22 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>-11.083</v>
+        <v>-23.441</v>
       </c>
       <c r="C91" t="n">
-        <v>1.465</v>
+        <v>1.94</v>
       </c>
       <c r="D91" t="n">
-        <v>0.919</v>
+        <v>1.859</v>
       </c>
       <c r="E91" t="n">
-        <v>0.959</v>
+        <v>1.363</v>
       </c>
       <c r="F91" t="n">
-        <v>0.904</v>
+        <v>1.363</v>
       </c>
       <c r="G91" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
@@ -2747,19 +2747,19 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>-7.082</v>
+        <v>-14.313</v>
       </c>
       <c r="C93" t="n">
-        <v>1.311</v>
+        <v>1.589</v>
       </c>
       <c r="D93" t="n">
-        <v>0.162</v>
+        <v>0.307</v>
       </c>
       <c r="E93" t="n">
-        <v>0.402</v>
+        <v>0.554</v>
       </c>
       <c r="F93" t="n">
-        <v>0.473</v>
+        <v>0.638</v>
       </c>
       <c r="G93" t="n">
         <v>1</v>
@@ -2772,19 +2772,19 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>-2.622</v>
+        <v>-12.861</v>
       </c>
       <c r="C94" t="n">
-        <v>1.139</v>
+        <v>1.533</v>
       </c>
       <c r="D94" t="n">
-        <v>0.073</v>
+        <v>0.278</v>
       </c>
       <c r="E94" t="n">
-        <v>0.27</v>
+        <v>0.527</v>
       </c>
       <c r="F94" t="n">
-        <v>0.316</v>
+        <v>0.665</v>
       </c>
       <c r="G94" t="n">
         <v>1</v>
@@ -2797,19 +2797,19 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>-31.01</v>
+        <v>-15.067</v>
       </c>
       <c r="C95" t="n">
-        <v>3.91</v>
+        <v>2.461</v>
       </c>
       <c r="D95" t="n">
-        <v>0.641</v>
+        <v>0.322</v>
       </c>
       <c r="E95" t="n">
-        <v>0.801</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="F95" t="n">
-        <v>0.801</v>
+        <v>0.555</v>
       </c>
       <c r="G95" t="n">
         <v>1</v>
@@ -2822,19 +2822,19 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>-28185.452</v>
+        <v>-28382.017</v>
       </c>
       <c r="C96" t="n">
-        <v>1085.094</v>
+        <v>1092.654</v>
       </c>
       <c r="D96" t="n">
-        <v>564.763</v>
+        <v>568.702</v>
       </c>
       <c r="E96" t="n">
-        <v>23.765</v>
+        <v>23.847</v>
       </c>
       <c r="F96" t="n">
-        <v>20.304</v>
+        <v>20.442</v>
       </c>
       <c r="G96" t="n">
         <v>-1</v>
@@ -2872,19 +2872,19 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>-2.465</v>
+        <v>-3.659</v>
       </c>
       <c r="C98" t="n">
-        <v>1.133</v>
+        <v>1.179</v>
       </c>
       <c r="D98" t="n">
-        <v>0.175</v>
+        <v>0.235</v>
       </c>
       <c r="E98" t="n">
-        <v>0.418</v>
+        <v>0.485</v>
       </c>
       <c r="F98" t="n">
-        <v>0.493</v>
+        <v>0.555</v>
       </c>
       <c r="G98" t="n">
         <v>1</v>
@@ -2897,19 +2897,19 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>-2.651</v>
+        <v>-42.184</v>
       </c>
       <c r="C99" t="n">
-        <v>1.14</v>
+        <v>2.661</v>
       </c>
       <c r="D99" t="n">
-        <v>0.184</v>
+        <v>2.18</v>
       </c>
       <c r="E99" t="n">
-        <v>0.429</v>
+        <v>1.476</v>
       </c>
       <c r="F99" t="n">
-        <v>0.4</v>
+        <v>1.469</v>
       </c>
       <c r="G99" t="n">
         <v>1</v>
@@ -2922,19 +2922,19 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>-6.427</v>
+        <v>-16.496</v>
       </c>
       <c r="C100" t="n">
-        <v>1.675</v>
+        <v>2.591</v>
       </c>
       <c r="D100" t="n">
-        <v>0.375</v>
+        <v>0.883</v>
       </c>
       <c r="E100" t="n">
-        <v>0.612</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="F100" t="n">
-        <v>0.449</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="G100" t="n">
         <v>-1</v>
@@ -2947,19 +2947,19 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>-53.121</v>
+        <v>-69.794</v>
       </c>
       <c r="C101" t="n">
-        <v>3.082</v>
+        <v>3.723</v>
       </c>
       <c r="D101" t="n">
-        <v>2.732</v>
+        <v>3.574</v>
       </c>
       <c r="E101" t="n">
-        <v>1.653</v>
+        <v>1.891</v>
       </c>
       <c r="F101" t="n">
-        <v>1.384</v>
+        <v>1.549</v>
       </c>
       <c r="G101" t="n">
         <v>1</v>
@@ -2997,19 +2997,19 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>-6.619</v>
+        <v>-7.489</v>
       </c>
       <c r="C103" t="n">
-        <v>1.293</v>
+        <v>1.326</v>
       </c>
       <c r="D103" t="n">
-        <v>0.238</v>
+        <v>0.265</v>
       </c>
       <c r="E103" t="n">
-        <v>0.488</v>
+        <v>0.515</v>
       </c>
       <c r="F103" t="n">
-        <v>0.474</v>
+        <v>0.51</v>
       </c>
       <c r="G103" t="n">
         <v>1</v>
@@ -3022,22 +3022,22 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>-36.86</v>
+        <v>-23.288</v>
       </c>
       <c r="C104" t="n">
-        <v>2.456</v>
+        <v>1.934</v>
       </c>
       <c r="D104" t="n">
-        <v>1.182</v>
+        <v>0.758</v>
       </c>
       <c r="E104" t="n">
-        <v>1.087</v>
+        <v>0.871</v>
       </c>
       <c r="F104" t="n">
-        <v>1.073</v>
+        <v>0.866</v>
       </c>
       <c r="G104" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -3047,19 +3047,19 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>-8.352</v>
+        <v>-8.936999999999999</v>
       </c>
       <c r="C105" t="n">
-        <v>1.85</v>
+        <v>1.903</v>
       </c>
       <c r="D105" t="n">
-        <v>0.292</v>
+        <v>0.31</v>
       </c>
       <c r="E105" t="n">
-        <v>0.54</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="F105" t="n">
-        <v>0.517</v>
+        <v>0.728</v>
       </c>
       <c r="G105" t="n">
         <v>1</v>
@@ -3072,19 +3072,19 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>-142.704</v>
+        <v>-104.547</v>
       </c>
       <c r="C106" t="n">
-        <v>6.527</v>
+        <v>5.06</v>
       </c>
       <c r="D106" t="n">
-        <v>4.487</v>
+        <v>3.295</v>
       </c>
       <c r="E106" t="n">
-        <v>2.118</v>
+        <v>1.815</v>
       </c>
       <c r="F106" t="n">
-        <v>1.941</v>
+        <v>1.691</v>
       </c>
       <c r="G106" t="n">
         <v>1</v>
@@ -3122,19 +3122,19 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>-51.237</v>
+        <v>-52.394</v>
       </c>
       <c r="C108" t="n">
-        <v>3.009</v>
+        <v>3.054</v>
       </c>
       <c r="D108" t="n">
-        <v>1.412</v>
+        <v>1.443</v>
       </c>
       <c r="E108" t="n">
-        <v>1.188</v>
+        <v>1.201</v>
       </c>
       <c r="F108" t="n">
-        <v>1.137</v>
+        <v>1.154</v>
       </c>
       <c r="G108" t="n">
         <v>-1</v>
@@ -3147,22 +3147,22 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>-80.191</v>
+        <v>-37.857</v>
       </c>
       <c r="C109" t="n">
-        <v>4.123</v>
+        <v>2.494</v>
       </c>
       <c r="D109" t="n">
-        <v>2.194</v>
+        <v>1.05</v>
       </c>
       <c r="E109" t="n">
-        <v>1.481</v>
+        <v>1.025</v>
       </c>
       <c r="F109" t="n">
-        <v>1.464</v>
+        <v>0.804</v>
       </c>
       <c r="G109" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="110">
@@ -3172,19 +3172,19 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>-20.701</v>
+        <v>-80.002</v>
       </c>
       <c r="C110" t="n">
-        <v>2.973</v>
+        <v>8.364000000000001</v>
       </c>
       <c r="D110" t="n">
-        <v>0.587</v>
+        <v>2.189</v>
       </c>
       <c r="E110" t="n">
-        <v>0.766</v>
+        <v>1.48</v>
       </c>
       <c r="F110" t="n">
-        <v>0.5600000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="G110" t="n">
         <v>-1</v>
@@ -3197,19 +3197,19 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>-39.223</v>
+        <v>-58.18</v>
       </c>
       <c r="C111" t="n">
-        <v>2.547</v>
+        <v>3.276</v>
       </c>
       <c r="D111" t="n">
-        <v>1.087</v>
+        <v>1.599</v>
       </c>
       <c r="E111" t="n">
-        <v>1.043</v>
+        <v>1.265</v>
       </c>
       <c r="F111" t="n">
-        <v>0.839</v>
+        <v>1.131</v>
       </c>
       <c r="G111" t="n">
         <v>-1</v>
@@ -3247,19 +3247,19 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>-88.52800000000001</v>
+        <v>-99.84699999999999</v>
       </c>
       <c r="C113" t="n">
-        <v>4.443</v>
+        <v>4.879</v>
       </c>
       <c r="D113" t="n">
-        <v>3.043</v>
+        <v>3.428</v>
       </c>
       <c r="E113" t="n">
-        <v>1.744</v>
+        <v>1.851</v>
       </c>
       <c r="F113" t="n">
-        <v>1.709</v>
+        <v>1.79</v>
       </c>
       <c r="G113" t="n">
         <v>1</v>
@@ -3272,19 +3272,19 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>-39.137</v>
+        <v>-24.664</v>
       </c>
       <c r="C114" t="n">
-        <v>2.544</v>
+        <v>1.987</v>
       </c>
       <c r="D114" t="n">
-        <v>1.364</v>
+        <v>0.872</v>
       </c>
       <c r="E114" t="n">
-        <v>1.168</v>
+        <v>0.9340000000000001</v>
       </c>
       <c r="F114" t="n">
-        <v>1.165</v>
+        <v>0.9330000000000001</v>
       </c>
       <c r="G114" t="n">
         <v>1</v>
@@ -3297,19 +3297,19 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>-63.035</v>
+        <v>-27.676</v>
       </c>
       <c r="C115" t="n">
-        <v>6.821</v>
+        <v>3.607</v>
       </c>
       <c r="D115" t="n">
-        <v>2.177</v>
+        <v>0.975</v>
       </c>
       <c r="E115" t="n">
-        <v>1.475</v>
+        <v>0.987</v>
       </c>
       <c r="F115" t="n">
-        <v>1.381</v>
+        <v>0.698</v>
       </c>
       <c r="G115" t="n">
         <v>-1</v>
@@ -3322,19 +3322,19 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>-41.748</v>
+        <v>-63.127</v>
       </c>
       <c r="C116" t="n">
-        <v>2.644</v>
+        <v>3.466</v>
       </c>
       <c r="D116" t="n">
-        <v>1.453</v>
+        <v>2.18</v>
       </c>
       <c r="E116" t="n">
-        <v>1.205</v>
+        <v>1.476</v>
       </c>
       <c r="F116" t="n">
-        <v>1.198</v>
+        <v>1.476</v>
       </c>
       <c r="G116" t="n">
         <v>1</v>
@@ -3372,19 +3372,19 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>-0.948</v>
+        <v>-1.164</v>
       </c>
       <c r="C118" t="n">
-        <v>1.075</v>
+        <v>1.083</v>
       </c>
       <c r="D118" t="n">
-        <v>0.308</v>
+        <v>0.342</v>
       </c>
       <c r="E118" t="n">
-        <v>0.555</v>
+        <v>0.585</v>
       </c>
       <c r="F118" t="n">
-        <v>0.628</v>
+        <v>0.613</v>
       </c>
       <c r="G118" t="n">
         <v>1</v>
@@ -3397,19 +3397,19 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>-8.553000000000001</v>
+        <v>-9.201000000000001</v>
       </c>
       <c r="C119" t="n">
-        <v>1.367</v>
+        <v>1.392</v>
       </c>
       <c r="D119" t="n">
-        <v>1.508</v>
+        <v>1.61</v>
       </c>
       <c r="E119" t="n">
-        <v>1.228</v>
+        <v>1.269</v>
       </c>
       <c r="F119" t="n">
-        <v>1.02</v>
+        <v>1.096</v>
       </c>
       <c r="G119" t="n">
         <v>-1</v>
@@ -3422,22 +3422,22 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>-0.6870000000000001</v>
+        <v>-0.264</v>
       </c>
       <c r="C120" t="n">
-        <v>1.153</v>
+        <v>1.115</v>
       </c>
       <c r="D120" t="n">
-        <v>0.266</v>
+        <v>0.2</v>
       </c>
       <c r="E120" t="n">
-        <v>0.516</v>
+        <v>0.447</v>
       </c>
       <c r="F120" t="n">
-        <v>0.397</v>
+        <v>0.426</v>
       </c>
       <c r="G120" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -3447,19 +3447,19 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>-1.272</v>
+        <v>-1.613</v>
       </c>
       <c r="C121" t="n">
-        <v>1.087</v>
+        <v>1.1</v>
       </c>
       <c r="D121" t="n">
-        <v>0.359</v>
+        <v>0.412</v>
       </c>
       <c r="E121" t="n">
-        <v>0.599</v>
+        <v>0.642</v>
       </c>
       <c r="F121" t="n">
-        <v>0.661</v>
+        <v>0.756</v>
       </c>
       <c r="G121" t="n">
         <v>1</v>
@@ -3497,19 +3497,19 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>-0.983</v>
+        <v>-0.88</v>
       </c>
       <c r="C123" t="n">
-        <v>1.076</v>
+        <v>1.072</v>
       </c>
       <c r="D123" t="n">
-        <v>1.3</v>
+        <v>1.232</v>
       </c>
       <c r="E123" t="n">
-        <v>1.14</v>
+        <v>1.11</v>
       </c>
       <c r="F123" t="n">
-        <v>1.314</v>
+        <v>1.164</v>
       </c>
       <c r="G123" t="n">
         <v>1</v>
@@ -3522,19 +3522,19 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>-0.018</v>
+        <v>-11.775</v>
       </c>
       <c r="C124" t="n">
-        <v>1.039</v>
+        <v>1.491</v>
       </c>
       <c r="D124" t="n">
-        <v>0.667</v>
+        <v>8.372</v>
       </c>
       <c r="E124" t="n">
-        <v>0.8169999999999999</v>
+        <v>2.893</v>
       </c>
       <c r="F124" t="n">
-        <v>0.8100000000000001</v>
+        <v>2.82</v>
       </c>
       <c r="G124" t="n">
         <v>1</v>
@@ -3547,19 +3547,19 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>-0.99</v>
+        <v>-0.78</v>
       </c>
       <c r="C125" t="n">
-        <v>1.181</v>
+        <v>1.162</v>
       </c>
       <c r="D125" t="n">
-        <v>1.304</v>
+        <v>1.167</v>
       </c>
       <c r="E125" t="n">
-        <v>1.142</v>
+        <v>1.08</v>
       </c>
       <c r="F125" t="n">
-        <v>1.03</v>
+        <v>1.323</v>
       </c>
       <c r="G125" t="n">
         <v>1</v>
@@ -3572,19 +3572,19 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>-0.5570000000000001</v>
+        <v>-0.963</v>
       </c>
       <c r="C126" t="n">
-        <v>1.06</v>
+        <v>1.076</v>
       </c>
       <c r="D126" t="n">
-        <v>1.02</v>
+        <v>1.286</v>
       </c>
       <c r="E126" t="n">
-        <v>1.01</v>
+        <v>1.134</v>
       </c>
       <c r="F126" t="n">
-        <v>1.038</v>
+        <v>1.036</v>
       </c>
       <c r="G126" t="n">
         <v>1</v>
@@ -3622,22 +3622,22 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>-9.93</v>
+        <v>-2.951</v>
       </c>
       <c r="C128" t="n">
-        <v>1.42</v>
+        <v>1.152</v>
       </c>
       <c r="D128" t="n">
-        <v>0.776</v>
+        <v>0.281</v>
       </c>
       <c r="E128" t="n">
-        <v>0.881</v>
+        <v>0.53</v>
       </c>
       <c r="F128" t="n">
-        <v>0.732</v>
+        <v>0.54</v>
       </c>
       <c r="G128" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129">
@@ -3647,19 +3647,19 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>-11.169</v>
+        <v>-20.002</v>
       </c>
       <c r="C129" t="n">
-        <v>1.468</v>
+        <v>1.808</v>
       </c>
       <c r="D129" t="n">
-        <v>0.864</v>
+        <v>1.492</v>
       </c>
       <c r="E129" t="n">
-        <v>0.93</v>
+        <v>1.221</v>
       </c>
       <c r="F129" t="n">
-        <v>0.924</v>
+        <v>1.095</v>
       </c>
       <c r="G129" t="n">
         <v>1</v>
@@ -3672,19 +3672,19 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>-1.406</v>
+        <v>-9.103</v>
       </c>
       <c r="C130" t="n">
-        <v>1.219</v>
+        <v>1.918</v>
       </c>
       <c r="D130" t="n">
-        <v>0.171</v>
+        <v>0.718</v>
       </c>
       <c r="E130" t="n">
-        <v>0.414</v>
+        <v>0.847</v>
       </c>
       <c r="F130" t="n">
-        <v>0.347</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="G130" t="n">
         <v>1</v>
@@ -3697,19 +3697,19 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>-2.04</v>
+        <v>-2.432</v>
       </c>
       <c r="C131" t="n">
-        <v>1.117</v>
+        <v>1.132</v>
       </c>
       <c r="D131" t="n">
-        <v>0.216</v>
+        <v>0.244</v>
       </c>
       <c r="E131" t="n">
-        <v>0.465</v>
+        <v>0.494</v>
       </c>
       <c r="F131" t="n">
-        <v>0.408</v>
+        <v>0.426</v>
       </c>
       <c r="G131" t="n">
         <v>1</v>
@@ -3747,19 +3747,19 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>-345.514</v>
+        <v>-270.672</v>
       </c>
       <c r="C133" t="n">
-        <v>14.327</v>
+        <v>11.449</v>
       </c>
       <c r="D133" t="n">
-        <v>3.758</v>
+        <v>2.947</v>
       </c>
       <c r="E133" t="n">
-        <v>1.939</v>
+        <v>1.717</v>
       </c>
       <c r="F133" t="n">
-        <v>1.937</v>
+        <v>1.706</v>
       </c>
       <c r="G133" t="n">
         <v>1</v>
@@ -3772,19 +3772,19 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>-247.914</v>
+        <v>-647.9400000000001</v>
       </c>
       <c r="C134" t="n">
-        <v>10.574</v>
+        <v>25.959</v>
       </c>
       <c r="D134" t="n">
-        <v>2.7</v>
+        <v>7.038</v>
       </c>
       <c r="E134" t="n">
-        <v>1.643</v>
+        <v>2.653</v>
       </c>
       <c r="F134" t="n">
-        <v>1.558</v>
+        <v>1.979</v>
       </c>
       <c r="G134" t="n">
         <v>1</v>
@@ -3797,19 +3797,19 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>-313.625</v>
+        <v>-965.818</v>
       </c>
       <c r="C135" t="n">
-        <v>29.602</v>
+        <v>88.893</v>
       </c>
       <c r="D135" t="n">
-        <v>3.412</v>
+        <v>10.486</v>
       </c>
       <c r="E135" t="n">
-        <v>1.847</v>
+        <v>3.238</v>
       </c>
       <c r="F135" t="n">
-        <v>1.479</v>
+        <v>2.7</v>
       </c>
       <c r="G135" t="n">
         <v>1</v>
@@ -3822,19 +3822,19 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>-1262.794</v>
+        <v>-1341.815</v>
       </c>
       <c r="C136" t="n">
-        <v>49.607</v>
+        <v>52.647</v>
       </c>
       <c r="D136" t="n">
-        <v>13.707</v>
+        <v>14.564</v>
       </c>
       <c r="E136" t="n">
-        <v>3.702</v>
+        <v>3.816</v>
       </c>
       <c r="F136" t="n">
-        <v>3.341</v>
+        <v>3.4</v>
       </c>
       <c r="G136" t="n">
         <v>1</v>
@@ -3872,22 +3872,22 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>-0.856</v>
+        <v>-0.802</v>
       </c>
       <c r="C138" t="n">
-        <v>1.071</v>
+        <v>1.069</v>
       </c>
       <c r="D138" t="n">
-        <v>2.348</v>
+        <v>2.279</v>
       </c>
       <c r="E138" t="n">
-        <v>1.532</v>
+        <v>1.51</v>
       </c>
       <c r="F138" t="n">
-        <v>1.125</v>
+        <v>1.191</v>
       </c>
       <c r="G138" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139">
@@ -3897,22 +3897,22 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>-0.541</v>
+        <v>-0.47</v>
       </c>
       <c r="C139" t="n">
-        <v>1.059</v>
+        <v>1.057</v>
       </c>
       <c r="D139" t="n">
-        <v>1.949</v>
+        <v>1.86</v>
       </c>
       <c r="E139" t="n">
-        <v>1.396</v>
+        <v>1.364</v>
       </c>
       <c r="F139" t="n">
         <v>1.125</v>
       </c>
       <c r="G139" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="140">
@@ -3922,19 +3922,19 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>-2.887</v>
+        <v>0.821</v>
       </c>
       <c r="C140" t="n">
-        <v>1.353</v>
+        <v>1.016</v>
       </c>
       <c r="D140" t="n">
-        <v>4.917</v>
+        <v>0.227</v>
       </c>
       <c r="E140" t="n">
-        <v>2.217</v>
+        <v>0.476</v>
       </c>
       <c r="F140" t="n">
-        <v>2.176</v>
+        <v>1.461</v>
       </c>
       <c r="G140" t="n">
         <v>1</v>
@@ -3947,19 +3947,19 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>-1.056</v>
+        <v>-0.8169999999999999</v>
       </c>
       <c r="C141" t="n">
-        <v>1.079</v>
+        <v>1.07</v>
       </c>
       <c r="D141" t="n">
-        <v>2.601</v>
+        <v>2.299</v>
       </c>
       <c r="E141" t="n">
-        <v>1.613</v>
+        <v>1.516</v>
       </c>
       <c r="F141" t="n">
-        <v>1.244</v>
+        <v>1.199</v>
       </c>
       <c r="G141" t="n">
         <v>1</v>
@@ -3997,19 +3997,19 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>-24.61</v>
+        <v>-24.15</v>
       </c>
       <c r="C143" t="n">
-        <v>1.985</v>
+        <v>1.967</v>
       </c>
       <c r="D143" t="n">
-        <v>3.949</v>
+        <v>3.878</v>
       </c>
       <c r="E143" t="n">
-        <v>1.987</v>
+        <v>1.969</v>
       </c>
       <c r="F143" t="n">
-        <v>1.977</v>
+        <v>1.963</v>
       </c>
       <c r="G143" t="n">
         <v>1</v>
@@ -4022,19 +4022,19 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>-47.577</v>
+        <v>-52.262</v>
       </c>
       <c r="C144" t="n">
-        <v>2.868</v>
+        <v>3.049</v>
       </c>
       <c r="D144" t="n">
-        <v>7.49</v>
+        <v>8.212999999999999</v>
       </c>
       <c r="E144" t="n">
-        <v>2.737</v>
+        <v>2.866</v>
       </c>
       <c r="F144" t="n">
-        <v>2.638</v>
+        <v>2.844</v>
       </c>
       <c r="G144" t="n">
         <v>1</v>
@@ -4047,19 +4047,19 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>-18.299</v>
+        <v>-25.964</v>
       </c>
       <c r="C145" t="n">
-        <v>2.754</v>
+        <v>3.451</v>
       </c>
       <c r="D145" t="n">
-        <v>2.976</v>
+        <v>4.158</v>
       </c>
       <c r="E145" t="n">
-        <v>1.725</v>
+        <v>2.039</v>
       </c>
       <c r="F145" t="n">
-        <v>1.517</v>
+        <v>1.983</v>
       </c>
       <c r="G145" t="n">
         <v>-1</v>
@@ -4072,19 +4072,19 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>-19.481</v>
+        <v>-13.775</v>
       </c>
       <c r="C146" t="n">
-        <v>1.788</v>
+        <v>1.568</v>
       </c>
       <c r="D146" t="n">
-        <v>3.158</v>
+        <v>2.278</v>
       </c>
       <c r="E146" t="n">
-        <v>1.777</v>
+        <v>1.509</v>
       </c>
       <c r="F146" t="n">
-        <v>1.775</v>
+        <v>1.496</v>
       </c>
       <c r="G146" t="n">
         <v>1</v>
@@ -4122,19 +4122,19 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>-3909.188</v>
+        <v>-3590.724</v>
       </c>
       <c r="C148" t="n">
-        <v>151.392</v>
+        <v>139.143</v>
       </c>
       <c r="D148" t="n">
-        <v>4.575</v>
+        <v>4.202</v>
       </c>
       <c r="E148" t="n">
-        <v>2.139</v>
+        <v>2.05</v>
       </c>
       <c r="F148" t="n">
-        <v>1.704</v>
+        <v>1.561</v>
       </c>
       <c r="G148" t="n">
         <v>1</v>
@@ -4147,19 +4147,19 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>-3809.02</v>
+        <v>-2792.564</v>
       </c>
       <c r="C149" t="n">
-        <v>147.539</v>
+        <v>108.445</v>
       </c>
       <c r="D149" t="n">
-        <v>4.458</v>
+        <v>3.268</v>
       </c>
       <c r="E149" t="n">
-        <v>2.111</v>
+        <v>1.808</v>
       </c>
       <c r="F149" t="n">
-        <v>1.991</v>
+        <v>1.696</v>
       </c>
       <c r="G149" t="n">
         <v>1</v>
@@ -4172,19 +4172,19 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>-2171.798</v>
+        <v>-1251.666</v>
       </c>
       <c r="C150" t="n">
-        <v>198.527</v>
+        <v>114.879</v>
       </c>
       <c r="D150" t="n">
-        <v>2.542</v>
+        <v>1.466</v>
       </c>
       <c r="E150" t="n">
-        <v>1.594</v>
+        <v>1.211</v>
       </c>
       <c r="F150" t="n">
-        <v>1.594</v>
+        <v>1.186</v>
       </c>
       <c r="G150" t="n">
         <v>1</v>
@@ -4197,19 +4197,19 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>-3219.447</v>
+        <v>-2881.665</v>
       </c>
       <c r="C151" t="n">
-        <v>124.863</v>
+        <v>111.872</v>
       </c>
       <c r="D151" t="n">
-        <v>3.768</v>
+        <v>3.373</v>
       </c>
       <c r="E151" t="n">
-        <v>1.941</v>
+        <v>1.837</v>
       </c>
       <c r="F151" t="n">
-        <v>1.666</v>
+        <v>1.446</v>
       </c>
       <c r="G151" t="n">
         <v>1</v>
@@ -4247,19 +4247,19 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>-8.417999999999999</v>
+        <v>-7.281</v>
       </c>
       <c r="C153" t="n">
-        <v>1.362</v>
+        <v>1.318</v>
       </c>
       <c r="D153" t="n">
-        <v>0.717</v>
+        <v>0.63</v>
       </c>
       <c r="E153" t="n">
-        <v>0.847</v>
+        <v>0.794</v>
       </c>
       <c r="F153" t="n">
-        <v>0.844</v>
+        <v>0.785</v>
       </c>
       <c r="G153" t="n">
         <v>1</v>
@@ -4272,22 +4272,22 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>-1.895</v>
+        <v>-51.328</v>
       </c>
       <c r="C154" t="n">
-        <v>1.111</v>
+        <v>3.013</v>
       </c>
       <c r="D154" t="n">
-        <v>0.22</v>
+        <v>3.983</v>
       </c>
       <c r="E154" t="n">
-        <v>0.469</v>
+        <v>1.996</v>
       </c>
       <c r="F154" t="n">
-        <v>0.716</v>
+        <v>1.966</v>
       </c>
       <c r="G154" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="155">
@@ -4297,22 +4297,22 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>-3.408</v>
+        <v>-28.7</v>
       </c>
       <c r="C155" t="n">
-        <v>1.401</v>
+        <v>3.7</v>
       </c>
       <c r="D155" t="n">
-        <v>0.335</v>
+        <v>2.26</v>
       </c>
       <c r="E155" t="n">
-        <v>0.579</v>
+        <v>1.503</v>
       </c>
       <c r="F155" t="n">
-        <v>0.631</v>
+        <v>1.218</v>
       </c>
       <c r="G155" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="156">
@@ -4322,19 +4322,19 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>0.057</v>
+        <v>0.126</v>
       </c>
       <c r="C156" t="n">
-        <v>1.036</v>
+        <v>1.034</v>
       </c>
       <c r="D156" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.066</v>
       </c>
       <c r="E156" t="n">
-        <v>0.268</v>
+        <v>0.257</v>
       </c>
       <c r="F156" t="n">
-        <v>0.276</v>
+        <v>0.311</v>
       </c>
       <c r="G156" t="n">
         <v>1</v>
@@ -4372,19 +4372,19 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>-27.677</v>
+        <v>-25.842</v>
       </c>
       <c r="C158" t="n">
-        <v>2.103</v>
+        <v>2.032</v>
       </c>
       <c r="D158" t="n">
-        <v>2.55</v>
+        <v>2.387</v>
       </c>
       <c r="E158" t="n">
-        <v>1.597</v>
+        <v>1.545</v>
       </c>
       <c r="F158" t="n">
-        <v>1.426</v>
+        <v>1.374</v>
       </c>
       <c r="G158" t="n">
         <v>1</v>
@@ -4397,19 +4397,19 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>-15.458</v>
+        <v>-42.255</v>
       </c>
       <c r="C159" t="n">
-        <v>1.633</v>
+        <v>2.664</v>
       </c>
       <c r="D159" t="n">
-        <v>1.464</v>
+        <v>3.847</v>
       </c>
       <c r="E159" t="n">
-        <v>1.21</v>
+        <v>1.961</v>
       </c>
       <c r="F159" t="n">
-        <v>1.176</v>
+        <v>1.991</v>
       </c>
       <c r="G159" t="n">
         <v>1</v>
@@ -4422,19 +4422,19 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>-85.855</v>
+        <v>-3.542</v>
       </c>
       <c r="C160" t="n">
-        <v>8.896000000000001</v>
+        <v>1.413</v>
       </c>
       <c r="D160" t="n">
-        <v>7.725</v>
+        <v>0.404</v>
       </c>
       <c r="E160" t="n">
-        <v>2.779</v>
+        <v>0.636</v>
       </c>
       <c r="F160" t="n">
-        <v>2.66</v>
+        <v>0.406</v>
       </c>
       <c r="G160" t="n">
         <v>-1</v>
@@ -4447,19 +4447,19 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>-11133.353</v>
+        <v>-11157.595</v>
       </c>
       <c r="C161" t="n">
-        <v>429.244</v>
+        <v>430.177</v>
       </c>
       <c r="D161" t="n">
-        <v>990.25</v>
+        <v>992.4059999999999</v>
       </c>
       <c r="E161" t="n">
-        <v>31.468</v>
+        <v>31.502</v>
       </c>
       <c r="F161" t="n">
-        <v>22.998</v>
+        <v>23.052</v>
       </c>
       <c r="G161" t="n">
         <v>-1</v>
@@ -4497,19 +4497,19 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>-16.393</v>
+        <v>-20.245</v>
       </c>
       <c r="C163" t="n">
-        <v>1.669</v>
+        <v>1.817</v>
       </c>
       <c r="D163" t="n">
-        <v>2.123</v>
+        <v>2.593</v>
       </c>
       <c r="E163" t="n">
-        <v>1.457</v>
+        <v>1.61</v>
       </c>
       <c r="F163" t="n">
-        <v>1.365</v>
+        <v>1.505</v>
       </c>
       <c r="G163" t="n">
         <v>-1</v>
@@ -4522,19 +4522,19 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>-26.591</v>
+        <v>-36.736</v>
       </c>
       <c r="C164" t="n">
-        <v>2.061</v>
+        <v>2.451</v>
       </c>
       <c r="D164" t="n">
-        <v>3.367</v>
+        <v>4.606</v>
       </c>
       <c r="E164" t="n">
-        <v>1.835</v>
+        <v>2.146</v>
       </c>
       <c r="F164" t="n">
-        <v>1.518</v>
+        <v>1.783</v>
       </c>
       <c r="G164" t="n">
         <v>-1</v>
@@ -4547,22 +4547,22 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>-3.041</v>
+        <v>-51.216</v>
       </c>
       <c r="C165" t="n">
-        <v>1.367</v>
+        <v>5.747</v>
       </c>
       <c r="D165" t="n">
-        <v>0.493</v>
+        <v>6.373</v>
       </c>
       <c r="E165" t="n">
-        <v>0.702</v>
+        <v>2.524</v>
       </c>
       <c r="F165" t="n">
-        <v>0.6860000000000001</v>
+        <v>1.775</v>
       </c>
       <c r="G165" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="166">
@@ -4572,19 +4572,19 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>-19.632</v>
+        <v>-16.833</v>
       </c>
       <c r="C166" t="n">
-        <v>1.794</v>
+        <v>1.686</v>
       </c>
       <c r="D166" t="n">
-        <v>2.518</v>
+        <v>2.177</v>
       </c>
       <c r="E166" t="n">
-        <v>1.587</v>
+        <v>1.475</v>
       </c>
       <c r="F166" t="n">
-        <v>1.37</v>
+        <v>1.215</v>
       </c>
       <c r="G166" t="n">
         <v>-1</v>
@@ -4622,22 +4622,22 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>0.1196666666666666</v>
+        <v>0.1087333333333333</v>
       </c>
       <c r="C168" t="n">
-        <v>1.4402</v>
+        <v>1.4456</v>
       </c>
       <c r="D168" t="n">
-        <v>0.8707999999999999</v>
+        <v>0.9013333333333333</v>
       </c>
       <c r="E168" t="n">
-        <v>0.8241333333333335</v>
+        <v>0.8348000000000001</v>
       </c>
       <c r="F168" t="n">
-        <v>0.8855333333333333</v>
+        <v>0.8901333333333333</v>
       </c>
       <c r="G168" t="n">
-        <v>0.5448000000000001</v>
+        <v>0.5486000000000001</v>
       </c>
     </row>
     <row r="169">
@@ -4647,22 +4647,22 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>-0.7838000000000001</v>
+        <v>-0.4467333333333333</v>
       </c>
       <c r="C169" t="n">
-        <v>3.5815</v>
+        <v>4.032733333333334</v>
       </c>
       <c r="D169" t="n">
-        <v>1.945866666666666</v>
+        <v>1.364233333333333</v>
       </c>
       <c r="E169" t="n">
-        <v>1.0501</v>
+        <v>0.9582333333333335</v>
       </c>
       <c r="F169" t="n">
-        <v>0.9734666666666666</v>
+        <v>0.9404666666666667</v>
       </c>
       <c r="G169" t="n">
-        <v>0.4588</v>
+        <v>0.4848</v>
       </c>
     </row>
     <row r="170">
@@ -4672,22 +4672,22 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>-0.3516</v>
+        <v>-0.8475333333333332</v>
       </c>
       <c r="C170" t="n">
-        <v>5.0548</v>
+        <v>6.542600000000001</v>
       </c>
       <c r="D170" t="n">
-        <v>1.580266666666667</v>
+        <v>1.8296</v>
       </c>
       <c r="E170" t="n">
-        <v>1.0034</v>
+        <v>1.062266666666667</v>
       </c>
       <c r="F170" t="n">
-        <v>0.9241333333333335</v>
+        <v>0.9644666666666666</v>
       </c>
       <c r="G170" t="n">
-        <v>0.4680666666666667</v>
+        <v>0.4757333333333333</v>
       </c>
     </row>
     <row r="171">
@@ -4697,22 +4697,22 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.1572666666666667</v>
+        <v>0.1926</v>
       </c>
       <c r="C171" t="n">
-        <v>1.421466666666667</v>
+        <v>1.4036</v>
       </c>
       <c r="D171" t="n">
-        <v>0.8438</v>
+        <v>0.8141333333333333</v>
       </c>
       <c r="E171" t="n">
-        <v>0.8083333333333333</v>
+        <v>0.7876000000000001</v>
       </c>
       <c r="F171" t="n">
-        <v>0.8797333333333331</v>
+        <v>0.8712666666666666</v>
       </c>
       <c r="G171" t="n">
-        <v>0.5577333333333333</v>
+        <v>0.5649333333333332</v>
       </c>
     </row>
     <row r="172">
@@ -4747,22 +4747,22 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>-250.4610555555556</v>
+        <v>-229.4286666666666</v>
       </c>
       <c r="C173" t="n">
-        <v>10.6715</v>
+        <v>9.862555555555556</v>
       </c>
       <c r="D173" t="n">
-        <v>1.773555555555556</v>
+        <v>1.711555555555555</v>
       </c>
       <c r="E173" t="n">
-        <v>1.201055555555556</v>
+        <v>1.182444444444444</v>
       </c>
       <c r="F173" t="n">
-        <v>1.158888888888889</v>
+        <v>1.141277777777778</v>
       </c>
       <c r="G173" t="n">
-        <v>0.4444444444444444</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="174">
@@ -4772,22 +4772,22 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>-204.9813611111111</v>
+        <v>-179.3878888888889</v>
       </c>
       <c r="C174" t="n">
-        <v>13.06955555555555</v>
+        <v>11.76422222222222</v>
       </c>
       <c r="D174" t="n">
-        <v>5.29736111111111</v>
+        <v>4.812555555555555</v>
       </c>
       <c r="E174" t="n">
-        <v>1.602972222222222</v>
+        <v>1.693916666666667</v>
       </c>
       <c r="F174" t="n">
-        <v>1.487694444444444</v>
+        <v>1.571388888888889</v>
       </c>
       <c r="G174" t="n">
-        <v>0.3888888888888889</v>
+        <v>0.2777777777777778</v>
       </c>
     </row>
     <row r="175">
@@ -4797,19 +4797,19 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>-157.1497222222222</v>
+        <v>-144.9055</v>
       </c>
       <c r="C175" t="n">
-        <v>15.37716666666667</v>
+        <v>14.26416666666667</v>
       </c>
       <c r="D175" t="n">
-        <v>3.627555555555555</v>
+        <v>5.980666666666667</v>
       </c>
       <c r="E175" t="n">
-        <v>1.501166666666667</v>
+        <v>1.630777777777777</v>
       </c>
       <c r="F175" t="n">
-        <v>1.374111111111111</v>
+        <v>1.500444444444444</v>
       </c>
       <c r="G175" t="n">
         <v>0.2222222222222222</v>
@@ -4822,22 +4822,22 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>-208944.6529444445</v>
+        <v>-208668.5283333334</v>
       </c>
       <c r="C176" t="n">
-        <v>8037.37122222222</v>
+        <v>8026.751111111111</v>
       </c>
       <c r="D176" t="n">
-        <v>106717.4843888889</v>
+        <v>106578.0088888889</v>
       </c>
       <c r="E176" t="n">
-        <v>112.874</v>
+        <v>112.8393888888889</v>
       </c>
       <c r="F176" t="n">
-        <v>91.36761111111112</v>
+        <v>91.35844444444443</v>
       </c>
       <c r="G176" t="n">
-        <v>0.2222222222222222</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="177">
@@ -4872,22 +4872,22 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>-41.64378703703704</v>
+        <v>-38.14749999999999</v>
       </c>
       <c r="C178" t="n">
-        <v>2.97875</v>
+        <v>2.848425925925925</v>
       </c>
       <c r="D178" t="n">
-        <v>1.021259259259259</v>
+        <v>1.03637037037037</v>
       </c>
       <c r="E178" t="n">
-        <v>0.8869537037037039</v>
+        <v>0.8927407407407407</v>
       </c>
       <c r="F178" t="n">
-        <v>0.9310925925925925</v>
+        <v>0.9319907407407407</v>
       </c>
       <c r="G178" t="n">
-        <v>0.5280740740740741</v>
+        <v>0.5682777777777778</v>
       </c>
     </row>
     <row r="179">
@@ -4897,22 +4897,22 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>-34.81672685185185</v>
+        <v>-30.27025925925926</v>
       </c>
       <c r="C179" t="n">
-        <v>5.162842592592592</v>
+        <v>5.321314814814815</v>
       </c>
       <c r="D179" t="n">
-        <v>2.504449074074074</v>
+        <v>1.938953703703704</v>
       </c>
       <c r="E179" t="n">
-        <v>1.142245370370371</v>
+        <v>1.080847222222222</v>
       </c>
       <c r="F179" t="n">
-        <v>1.059171296296296</v>
+        <v>1.04562037037037</v>
       </c>
       <c r="G179" t="n">
-        <v>0.4471481481481481</v>
+        <v>0.4502962962962963</v>
       </c>
     </row>
     <row r="180">
@@ -4922,22 +4922,22 @@
         </is>
       </c>
       <c r="B180" t="n">
-        <v>-26.48462037037038</v>
+        <v>-24.85719444444444</v>
       </c>
       <c r="C180" t="n">
-        <v>6.775194444444445</v>
+        <v>7.82952777777778</v>
       </c>
       <c r="D180" t="n">
-        <v>1.921481481481481</v>
+        <v>2.521444444444445</v>
       </c>
       <c r="E180" t="n">
-        <v>1.086361111111111</v>
+        <v>1.157018518518518</v>
       </c>
       <c r="F180" t="n">
-        <v>0.9991296296296298</v>
+        <v>1.053796296296296</v>
       </c>
       <c r="G180" t="n">
-        <v>0.4270925925925926</v>
+        <v>0.4334814814814814</v>
       </c>
     </row>
     <row r="181">
@@ -4947,22 +4947,22 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>-34823.97776851853</v>
+        <v>-34777.92755555557</v>
       </c>
       <c r="C181" t="n">
-        <v>1340.746425925926</v>
+        <v>1338.961518518518</v>
       </c>
       <c r="D181" t="n">
-        <v>17786.95056481481</v>
+        <v>17763.67992592593</v>
       </c>
       <c r="E181" t="n">
-        <v>19.48594444444445</v>
+        <v>19.46289814814815</v>
       </c>
       <c r="F181" t="n">
-        <v>15.9610462962963</v>
+        <v>15.95246296296296</v>
       </c>
       <c r="G181" t="n">
-        <v>0.5018148148148148</v>
+        <v>0.5263333333333332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated walk forward windows, added plots removing LR and Ensemble
</commit_message>
<xml_diff>
--- a/Brent3COVIDMetrics/rollingTestMetrics.xlsx
+++ b/Brent3COVIDMetrics/rollingTestMetrics.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G181"/>
+  <dimension ref="A1:G176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,22 +497,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.169</v>
+        <v>0.171</v>
       </c>
       <c r="C3" t="n">
-        <v>1.416</v>
+        <v>1.414</v>
       </c>
       <c r="D3" t="n">
-        <v>5.737</v>
+        <v>5.724</v>
       </c>
       <c r="E3" t="n">
-        <v>2.395</v>
+        <v>2.392</v>
       </c>
       <c r="F3" t="n">
         <v>2.26</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8070000000000001</v>
+        <v>0.725</v>
       </c>
     </row>
     <row r="4">
@@ -522,22 +522,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.453</v>
+        <v>0.481</v>
       </c>
       <c r="C4" t="n">
-        <v>1.273</v>
+        <v>1.26</v>
       </c>
       <c r="D4" t="n">
-        <v>3.776</v>
+        <v>3.584</v>
       </c>
       <c r="E4" t="n">
-        <v>1.943</v>
+        <v>1.893</v>
       </c>
       <c r="F4" t="n">
-        <v>2.674</v>
+        <v>2.372</v>
       </c>
       <c r="G4" t="n">
-        <v>0.698</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="5">
@@ -547,22 +547,22 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.139</v>
+        <v>-0.208</v>
       </c>
       <c r="C5" t="n">
-        <v>3.583</v>
+        <v>4.624</v>
       </c>
       <c r="D5" t="n">
-        <v>5.943</v>
+        <v>8.34</v>
       </c>
       <c r="E5" t="n">
-        <v>2.438</v>
+        <v>2.888</v>
       </c>
       <c r="F5" t="n">
-        <v>2.291</v>
+        <v>2.321</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="6">
@@ -572,22 +572,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.211</v>
+        <v>0.244</v>
       </c>
       <c r="C6" t="n">
-        <v>1.394</v>
+        <v>1.378</v>
       </c>
       <c r="D6" t="n">
-        <v>5.446</v>
+        <v>5.214</v>
       </c>
       <c r="E6" t="n">
-        <v>2.334</v>
+        <v>2.283</v>
       </c>
       <c r="F6" t="n">
-        <v>2.285</v>
+        <v>2.29</v>
       </c>
       <c r="G6" t="n">
-        <v>0.764</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="7">
@@ -622,22 +622,22 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.112</v>
+        <v>-0.083</v>
       </c>
       <c r="C8" t="n">
-        <v>1.556</v>
+        <v>1.542</v>
       </c>
       <c r="D8" t="n">
-        <v>0.706</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="E8" t="n">
-        <v>0.84</v>
+        <v>0.829</v>
       </c>
       <c r="F8" t="n">
-        <v>0.681</v>
+        <v>0.658</v>
       </c>
       <c r="G8" t="n">
-        <v>0.155</v>
+        <v>0.138</v>
       </c>
     </row>
     <row r="9">
@@ -647,22 +647,22 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.021</v>
+        <v>-1.194</v>
       </c>
       <c r="C9" t="n">
-        <v>1.49</v>
+        <v>2.097</v>
       </c>
       <c r="D9" t="n">
-        <v>0.622</v>
+        <v>1.393</v>
       </c>
       <c r="E9" t="n">
-        <v>0.789</v>
+        <v>1.18</v>
       </c>
       <c r="F9" t="n">
-        <v>0.664</v>
+        <v>0.904</v>
       </c>
       <c r="G9" t="n">
-        <v>0.278</v>
+        <v>-0.154</v>
       </c>
     </row>
     <row r="10">
@@ -672,22 +672,22 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.925</v>
+        <v>-0.592</v>
       </c>
       <c r="C10" t="n">
-        <v>6.775</v>
+        <v>5.776</v>
       </c>
       <c r="D10" t="n">
-        <v>1.223</v>
+        <v>1.011</v>
       </c>
       <c r="E10" t="n">
-        <v>1.106</v>
+        <v>1.005</v>
       </c>
       <c r="F10" t="n">
-        <v>0.882</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="G10" t="n">
-        <v>0.104</v>
+        <v>-0.162</v>
       </c>
     </row>
     <row r="11">
@@ -697,22 +697,22 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.066</v>
+        <v>-0.32</v>
       </c>
       <c r="C11" t="n">
-        <v>1.533</v>
+        <v>1.66</v>
       </c>
       <c r="D11" t="n">
-        <v>0.677</v>
+        <v>0.839</v>
       </c>
       <c r="E11" t="n">
-        <v>0.823</v>
+        <v>0.916</v>
       </c>
       <c r="F11" t="n">
-        <v>0.707</v>
+        <v>0.774</v>
       </c>
       <c r="G11" t="n">
-        <v>0.227</v>
+        <v>0.151</v>
       </c>
     </row>
     <row r="12">
@@ -747,22 +747,22 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-1.178</v>
+        <v>-0.887</v>
       </c>
       <c r="C13" t="n">
-        <v>2.089</v>
+        <v>1.944</v>
       </c>
       <c r="D13" t="n">
-        <v>0.38</v>
+        <v>0.329</v>
       </c>
       <c r="E13" t="n">
-        <v>0.616</v>
+        <v>0.574</v>
       </c>
       <c r="F13" t="n">
-        <v>0.521</v>
+        <v>0.49</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.049</v>
+        <v>-0.041</v>
       </c>
     </row>
     <row r="14">
@@ -772,22 +772,22 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-2.074</v>
+        <v>-0.922</v>
       </c>
       <c r="C14" t="n">
-        <v>2.537</v>
+        <v>1.961</v>
       </c>
       <c r="D14" t="n">
-        <v>0.536</v>
+        <v>0.335</v>
       </c>
       <c r="E14" t="n">
-        <v>0.732</v>
+        <v>0.579</v>
       </c>
       <c r="F14" t="n">
-        <v>0.629</v>
+        <v>0.495</v>
       </c>
       <c r="G14" t="n">
-        <v>0.204</v>
+        <v>0.083</v>
       </c>
     </row>
     <row r="15">
@@ -797,22 +797,22 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-1.181</v>
+        <v>-0.554</v>
       </c>
       <c r="C15" t="n">
-        <v>7.543</v>
+        <v>5.662</v>
       </c>
       <c r="D15" t="n">
-        <v>0.381</v>
+        <v>0.271</v>
       </c>
       <c r="E15" t="n">
-        <v>0.617</v>
+        <v>0.521</v>
       </c>
       <c r="F15" t="n">
-        <v>0.551</v>
+        <v>0.555</v>
       </c>
       <c r="G15" t="n">
-        <v>0.047</v>
+        <v>0.608</v>
       </c>
     </row>
     <row r="16">
@@ -822,22 +822,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-1.176</v>
+        <v>-1.052</v>
       </c>
       <c r="C16" t="n">
-        <v>2.088</v>
+        <v>2.026</v>
       </c>
       <c r="D16" t="n">
-        <v>0.38</v>
+        <v>0.358</v>
       </c>
       <c r="E16" t="n">
-        <v>0.616</v>
+        <v>0.598</v>
       </c>
       <c r="F16" t="n">
-        <v>0.453</v>
+        <v>0.478</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.183</v>
+        <v>-0.044</v>
       </c>
     </row>
     <row r="17">
@@ -872,22 +872,22 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.187</v>
+        <v>-0.053</v>
       </c>
       <c r="C18" t="n">
-        <v>1.406</v>
+        <v>1.526</v>
       </c>
       <c r="D18" t="n">
-        <v>0.639</v>
+        <v>0.827</v>
       </c>
       <c r="E18" t="n">
-        <v>0.799</v>
+        <v>0.909</v>
       </c>
       <c r="F18" t="n">
-        <v>0.911</v>
+        <v>0.958</v>
       </c>
       <c r="G18" t="n">
-        <v>0.643</v>
+        <v>0.613</v>
       </c>
     </row>
     <row r="19">
@@ -897,22 +897,22 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.279</v>
+        <v>-0.103</v>
       </c>
       <c r="C19" t="n">
-        <v>1.36</v>
+        <v>1.551</v>
       </c>
       <c r="D19" t="n">
-        <v>0.5669999999999999</v>
+        <v>0.867</v>
       </c>
       <c r="E19" t="n">
-        <v>0.753</v>
+        <v>0.931</v>
       </c>
       <c r="F19" t="n">
-        <v>0.801</v>
+        <v>0.851</v>
       </c>
       <c r="G19" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.5570000000000001</v>
       </c>
     </row>
     <row r="20">
@@ -922,22 +922,22 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.406</v>
+        <v>0.508</v>
       </c>
       <c r="C20" t="n">
-        <v>2.782</v>
+        <v>2.476</v>
       </c>
       <c r="D20" t="n">
-        <v>0.467</v>
+        <v>0.386</v>
       </c>
       <c r="E20" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.621</v>
       </c>
       <c r="F20" t="n">
-        <v>0.8080000000000001</v>
+        <v>0.78</v>
       </c>
       <c r="G20" t="n">
-        <v>0.716</v>
+        <v>0.856</v>
       </c>
     </row>
     <row r="21">
@@ -947,22 +947,22 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.209</v>
+        <v>0.062</v>
       </c>
       <c r="C21" t="n">
-        <v>1.396</v>
+        <v>1.469</v>
       </c>
       <c r="D21" t="n">
-        <v>0.622</v>
+        <v>0.737</v>
       </c>
       <c r="E21" t="n">
-        <v>0.789</v>
+        <v>0.858</v>
       </c>
       <c r="F21" t="n">
-        <v>0.833</v>
+        <v>0.905</v>
       </c>
       <c r="G21" t="n">
-        <v>0.627</v>
+        <v>0.602</v>
       </c>
     </row>
     <row r="22">
@@ -997,22 +997,22 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.23</v>
+        <v>0.216</v>
       </c>
       <c r="C23" t="n">
-        <v>1.385</v>
+        <v>1.392</v>
       </c>
       <c r="D23" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.695</v>
       </c>
       <c r="E23" t="n">
-        <v>0.826</v>
+        <v>0.834</v>
       </c>
       <c r="F23" t="n">
-        <v>0.946</v>
+        <v>0.9360000000000001</v>
       </c>
       <c r="G23" t="n">
-        <v>0.64</v>
+        <v>0.619</v>
       </c>
     </row>
     <row r="24">
@@ -1022,22 +1022,22 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.162</v>
+        <v>0.478</v>
       </c>
       <c r="C24" t="n">
-        <v>1.419</v>
+        <v>1.261</v>
       </c>
       <c r="D24" t="n">
-        <v>0.743</v>
+        <v>0.462</v>
       </c>
       <c r="E24" t="n">
-        <v>0.862</v>
+        <v>0.68</v>
       </c>
       <c r="F24" t="n">
-        <v>0.97</v>
+        <v>0.986</v>
       </c>
       <c r="G24" t="n">
-        <v>0.507</v>
+        <v>0.767</v>
       </c>
     </row>
     <row r="25">
@@ -1047,22 +1047,22 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.239</v>
+        <v>-0.146</v>
       </c>
       <c r="C25" t="n">
-        <v>3.283</v>
+        <v>4.438</v>
       </c>
       <c r="D25" t="n">
-        <v>0.675</v>
+        <v>1.016</v>
       </c>
       <c r="E25" t="n">
-        <v>0.822</v>
+        <v>1.008</v>
       </c>
       <c r="F25" t="n">
-        <v>1.014</v>
+        <v>1.07</v>
       </c>
       <c r="G25" t="n">
-        <v>0.643</v>
+        <v>0.547</v>
       </c>
     </row>
     <row r="26">
@@ -1072,22 +1072,22 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.295</v>
+        <v>0.287</v>
       </c>
       <c r="C26" t="n">
-        <v>1.352</v>
+        <v>1.356</v>
       </c>
       <c r="D26" t="n">
-        <v>0.625</v>
+        <v>0.632</v>
       </c>
       <c r="E26" t="n">
-        <v>0.791</v>
+        <v>0.795</v>
       </c>
       <c r="F26" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.9350000000000001</v>
       </c>
       <c r="G26" t="n">
-        <v>0.619</v>
+        <v>0.623</v>
       </c>
     </row>
     <row r="27">
@@ -1122,22 +1122,22 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.242</v>
+        <v>0.218</v>
       </c>
       <c r="C28" t="n">
-        <v>1.379</v>
+        <v>1.391</v>
       </c>
       <c r="D28" t="n">
-        <v>0.95</v>
+        <v>0.98</v>
       </c>
       <c r="E28" t="n">
-        <v>0.975</v>
+        <v>0.99</v>
       </c>
       <c r="F28" t="n">
-        <v>1.048</v>
+        <v>1.047</v>
       </c>
       <c r="G28" t="n">
-        <v>0.569</v>
+        <v>0.514</v>
       </c>
     </row>
     <row r="29">
@@ -1147,22 +1147,22 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.34</v>
+        <v>0.396</v>
       </c>
       <c r="C29" t="n">
-        <v>1.33</v>
+        <v>1.302</v>
       </c>
       <c r="D29" t="n">
-        <v>0.827</v>
+        <v>0.757</v>
       </c>
       <c r="E29" t="n">
-        <v>0.909</v>
+        <v>0.87</v>
       </c>
       <c r="F29" t="n">
-        <v>1.031</v>
+        <v>1.046</v>
       </c>
       <c r="G29" t="n">
-        <v>0.604</v>
+        <v>0.727</v>
       </c>
     </row>
     <row r="30">
@@ -1172,22 +1172,22 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.1</v>
+        <v>0.348</v>
       </c>
       <c r="C30" t="n">
-        <v>3.7</v>
+        <v>2.956</v>
       </c>
       <c r="D30" t="n">
-        <v>1.127</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="E30" t="n">
-        <v>1.062</v>
+        <v>0.904</v>
       </c>
       <c r="F30" t="n">
-        <v>1.106</v>
+        <v>1.054</v>
       </c>
       <c r="G30" t="n">
-        <v>0.547</v>
+        <v>0.6919999999999999</v>
       </c>
     </row>
     <row r="31">
@@ -1197,22 +1197,22 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.313</v>
+        <v>0.383</v>
       </c>
       <c r="C31" t="n">
-        <v>1.344</v>
+        <v>1.308</v>
       </c>
       <c r="D31" t="n">
-        <v>0.861</v>
+        <v>0.773</v>
       </c>
       <c r="E31" t="n">
-        <v>0.928</v>
+        <v>0.879</v>
       </c>
       <c r="F31" t="n">
-        <v>1.033</v>
+        <v>1.027</v>
       </c>
       <c r="G31" t="n">
-        <v>0.586</v>
+        <v>0.673</v>
       </c>
     </row>
     <row r="32">
@@ -1247,22 +1247,22 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.143</v>
+        <v>-0.116</v>
       </c>
       <c r="C33" t="n">
-        <v>1.428</v>
+        <v>1.558</v>
       </c>
       <c r="D33" t="n">
-        <v>0.294</v>
+        <v>0.383</v>
       </c>
       <c r="E33" t="n">
-        <v>0.542</v>
+        <v>0.619</v>
       </c>
       <c r="F33" t="n">
-        <v>0.592</v>
+        <v>0.581</v>
       </c>
       <c r="G33" t="n">
-        <v>0.577</v>
+        <v>0.345</v>
       </c>
     </row>
     <row r="34">
@@ -1272,22 +1272,22 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.063</v>
+        <v>-0.172</v>
       </c>
       <c r="C34" t="n">
-        <v>1.468</v>
+        <v>1.586</v>
       </c>
       <c r="D34" t="n">
-        <v>0.321</v>
+        <v>0.402</v>
       </c>
       <c r="E34" t="n">
-        <v>0.5669999999999999</v>
+        <v>0.634</v>
       </c>
       <c r="F34" t="n">
-        <v>0.6919999999999999</v>
+        <v>0.767</v>
       </c>
       <c r="G34" t="n">
-        <v>0.62</v>
+        <v>0.712</v>
       </c>
     </row>
     <row r="35">
@@ -1297,22 +1297,22 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-0.062</v>
+        <v>-0.376</v>
       </c>
       <c r="C35" t="n">
-        <v>4.186</v>
+        <v>5.128</v>
       </c>
       <c r="D35" t="n">
-        <v>0.364</v>
+        <v>0.472</v>
       </c>
       <c r="E35" t="n">
-        <v>0.603</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="F35" t="n">
-        <v>0.665</v>
+        <v>0.671</v>
       </c>
       <c r="G35" t="n">
-        <v>0.596</v>
+        <v>0.492</v>
       </c>
     </row>
     <row r="36">
@@ -1322,22 +1322,22 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.191</v>
+        <v>0.256</v>
       </c>
       <c r="C36" t="n">
-        <v>1.404</v>
+        <v>1.372</v>
       </c>
       <c r="D36" t="n">
-        <v>0.277</v>
+        <v>0.255</v>
       </c>
       <c r="E36" t="n">
-        <v>0.526</v>
+        <v>0.505</v>
       </c>
       <c r="F36" t="n">
-        <v>0.5639999999999999</v>
+        <v>0.5590000000000001</v>
       </c>
       <c r="G36" t="n">
-        <v>0.516</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="37">
@@ -1372,22 +1372,22 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.248</v>
+        <v>0.201</v>
       </c>
       <c r="C38" t="n">
-        <v>1.376</v>
+        <v>1.4</v>
       </c>
       <c r="D38" t="n">
-        <v>0.878</v>
+        <v>0.931</v>
       </c>
       <c r="E38" t="n">
-        <v>0.9370000000000001</v>
+        <v>0.965</v>
       </c>
       <c r="F38" t="n">
         <v>0.972</v>
       </c>
       <c r="G38" t="n">
-        <v>0.744</v>
+        <v>0.712</v>
       </c>
     </row>
     <row r="39">
@@ -1397,22 +1397,22 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.415</v>
+        <v>0.208</v>
       </c>
       <c r="C39" t="n">
-        <v>1.292</v>
+        <v>1.396</v>
       </c>
       <c r="D39" t="n">
-        <v>0.6820000000000001</v>
+        <v>0.923</v>
       </c>
       <c r="E39" t="n">
-        <v>0.826</v>
+        <v>0.961</v>
       </c>
       <c r="F39" t="n">
-        <v>0.952</v>
+        <v>0.996</v>
       </c>
       <c r="G39" t="n">
-        <v>0.852</v>
+        <v>0.478</v>
       </c>
     </row>
     <row r="40">
@@ -1422,22 +1422,22 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.205</v>
+        <v>0.345</v>
       </c>
       <c r="C40" t="n">
-        <v>3.385</v>
+        <v>2.965</v>
       </c>
       <c r="D40" t="n">
-        <v>0.927</v>
+        <v>0.764</v>
       </c>
       <c r="E40" t="n">
-        <v>0.963</v>
+        <v>0.874</v>
       </c>
       <c r="F40" t="n">
-        <v>0.999</v>
+        <v>0.956</v>
       </c>
       <c r="G40" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.835</v>
       </c>
     </row>
     <row r="41">
@@ -1447,22 +1447,22 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.276</v>
+        <v>0.366</v>
       </c>
       <c r="C41" t="n">
-        <v>1.362</v>
+        <v>1.317</v>
       </c>
       <c r="D41" t="n">
-        <v>0.845</v>
+        <v>0.74</v>
       </c>
       <c r="E41" t="n">
-        <v>0.919</v>
+        <v>0.86</v>
       </c>
       <c r="F41" t="n">
-        <v>0.97</v>
+        <v>0.982</v>
       </c>
       <c r="G41" t="n">
-        <v>0.8</v>
+        <v>0.859</v>
       </c>
     </row>
     <row r="42">
@@ -1497,22 +1497,22 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.469</v>
+        <v>0.39</v>
       </c>
       <c r="C43" t="n">
-        <v>1.266</v>
+        <v>1.305</v>
       </c>
       <c r="D43" t="n">
-        <v>0.476</v>
+        <v>0.547</v>
       </c>
       <c r="E43" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.915</v>
+      </c>
+      <c r="G43" t="n">
         <v>0.6899999999999999</v>
-      </c>
-      <c r="F43" t="n">
-        <v>0.904</v>
-      </c>
-      <c r="G43" t="n">
-        <v>0.756</v>
       </c>
     </row>
     <row r="44">
@@ -1522,22 +1522,22 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.264</v>
+        <v>0.27</v>
       </c>
       <c r="C44" t="n">
-        <v>1.368</v>
+        <v>1.365</v>
       </c>
       <c r="D44" t="n">
-        <v>0.659</v>
+        <v>0.654</v>
       </c>
       <c r="E44" t="n">
-        <v>0.8120000000000001</v>
+        <v>0.8090000000000001</v>
       </c>
       <c r="F44" t="n">
-        <v>0.856</v>
+        <v>0.972</v>
       </c>
       <c r="G44" t="n">
-        <v>0.595</v>
+        <v>0.555</v>
       </c>
     </row>
     <row r="45">
@@ -1547,22 +1547,22 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.045</v>
+        <v>0.006</v>
       </c>
       <c r="C45" t="n">
-        <v>3.865</v>
+        <v>3.982</v>
       </c>
       <c r="D45" t="n">
-        <v>0.856</v>
+        <v>0.891</v>
       </c>
       <c r="E45" t="n">
-        <v>0.925</v>
+        <v>0.944</v>
       </c>
       <c r="F45" t="n">
-        <v>0.852</v>
+        <v>0.853</v>
       </c>
       <c r="G45" t="n">
-        <v>0.229</v>
+        <v>0.193</v>
       </c>
     </row>
     <row r="46">
@@ -1572,22 +1572,22 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.543</v>
+        <v>0.503</v>
       </c>
       <c r="C46" t="n">
-        <v>1.228</v>
+        <v>1.248</v>
       </c>
       <c r="D46" t="n">
-        <v>0.41</v>
+        <v>0.445</v>
       </c>
       <c r="E46" t="n">
-        <v>0.64</v>
+        <v>0.667</v>
       </c>
       <c r="F46" t="n">
-        <v>0.88</v>
+        <v>0.929</v>
       </c>
       <c r="G46" t="n">
-        <v>0.8070000000000001</v>
+        <v>0.729</v>
       </c>
     </row>
     <row r="47">
@@ -1622,22 +1622,22 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.227</v>
+        <v>0.256</v>
       </c>
       <c r="C48" t="n">
-        <v>1.386</v>
+        <v>1.372</v>
       </c>
       <c r="D48" t="n">
-        <v>0.488</v>
+        <v>0.469</v>
       </c>
       <c r="E48" t="n">
-        <v>0.699</v>
+        <v>0.6850000000000001</v>
       </c>
       <c r="F48" t="n">
-        <v>0.851</v>
+        <v>0.85</v>
       </c>
       <c r="G48" t="n">
-        <v>0.631</v>
+        <v>0.637</v>
       </c>
     </row>
     <row r="49">
@@ -1647,22 +1647,22 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.354</v>
+        <v>0.417</v>
       </c>
       <c r="C49" t="n">
-        <v>1.323</v>
+        <v>1.292</v>
       </c>
       <c r="D49" t="n">
-        <v>0.408</v>
+        <v>0.367</v>
       </c>
       <c r="E49" t="n">
-        <v>0.639</v>
+        <v>0.606</v>
       </c>
       <c r="F49" t="n">
-        <v>0.765</v>
+        <v>0.889</v>
       </c>
       <c r="G49" t="n">
-        <v>0.6</v>
+        <v>0.705</v>
       </c>
     </row>
     <row r="50">
@@ -1672,22 +1672,22 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.442</v>
+        <v>0.329</v>
       </c>
       <c r="C50" t="n">
-        <v>2.674</v>
+        <v>3.013</v>
       </c>
       <c r="D50" t="n">
-        <v>0.352</v>
+        <v>0.423</v>
       </c>
       <c r="E50" t="n">
-        <v>0.593</v>
+        <v>0.65</v>
       </c>
       <c r="F50" t="n">
-        <v>0.713</v>
+        <v>0.725</v>
       </c>
       <c r="G50" t="n">
-        <v>0.84</v>
+        <v>0.629</v>
       </c>
     </row>
     <row r="51">
@@ -1697,22 +1697,22 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.446</v>
+        <v>0.317</v>
       </c>
       <c r="C51" t="n">
-        <v>1.277</v>
+        <v>1.342</v>
       </c>
       <c r="D51" t="n">
-        <v>0.35</v>
+        <v>0.431</v>
       </c>
       <c r="E51" t="n">
-        <v>0.592</v>
+        <v>0.657</v>
       </c>
       <c r="F51" t="n">
-        <v>0.792</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="G51" t="n">
-        <v>0.707</v>
+        <v>0.634</v>
       </c>
     </row>
     <row r="52">
@@ -1747,22 +1747,22 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.186</v>
+        <v>0.223</v>
       </c>
       <c r="C53" t="n">
-        <v>1.407</v>
+        <v>1.388</v>
       </c>
       <c r="D53" t="n">
-        <v>0.246</v>
+        <v>0.235</v>
       </c>
       <c r="E53" t="n">
-        <v>0.496</v>
+        <v>0.485</v>
       </c>
       <c r="F53" t="n">
-        <v>0.551</v>
+        <v>0.546</v>
       </c>
       <c r="G53" t="n">
-        <v>0.511</v>
+        <v>0.532</v>
       </c>
     </row>
     <row r="54">
@@ -1772,22 +1772,22 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.537</v>
+        <v>0.292</v>
       </c>
       <c r="C54" t="n">
-        <v>1.232</v>
+        <v>1.354</v>
       </c>
       <c r="D54" t="n">
-        <v>0.14</v>
+        <v>0.214</v>
       </c>
       <c r="E54" t="n">
-        <v>0.374</v>
+        <v>0.463</v>
       </c>
       <c r="F54" t="n">
-        <v>0.569</v>
+        <v>0.704</v>
       </c>
       <c r="G54" t="n">
-        <v>0.746</v>
+        <v>0.751</v>
       </c>
     </row>
     <row r="55">
@@ -1797,22 +1797,22 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>-0.641</v>
+        <v>-0.605</v>
       </c>
       <c r="C55" t="n">
-        <v>5.923</v>
+        <v>5.815</v>
       </c>
       <c r="D55" t="n">
-        <v>0.496</v>
+        <v>0.485</v>
       </c>
       <c r="E55" t="n">
-        <v>0.704</v>
+        <v>0.696</v>
       </c>
       <c r="F55" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.672</v>
       </c>
       <c r="G55" t="n">
-        <v>0.32</v>
+        <v>0.333</v>
       </c>
     </row>
     <row r="56">
@@ -1822,22 +1822,22 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.247</v>
+        <v>0.105</v>
       </c>
       <c r="C56" t="n">
-        <v>1.376</v>
+        <v>1.448</v>
       </c>
       <c r="D56" t="n">
-        <v>0.227</v>
+        <v>0.27</v>
       </c>
       <c r="E56" t="n">
-        <v>0.476</v>
+        <v>0.52</v>
       </c>
       <c r="F56" t="n">
-        <v>0.549</v>
+        <v>0.542</v>
       </c>
       <c r="G56" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.458</v>
       </c>
     </row>
     <row r="57">
@@ -1872,22 +1872,22 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>-0.181</v>
+        <v>-0.229</v>
       </c>
       <c r="C58" t="n">
-        <v>1.59</v>
+        <v>1.614</v>
       </c>
       <c r="D58" t="n">
-        <v>0.576</v>
+        <v>0.6</v>
       </c>
       <c r="E58" t="n">
-        <v>0.759</v>
+        <v>0.775</v>
       </c>
       <c r="F58" t="n">
-        <v>0.747</v>
+        <v>0.739</v>
       </c>
       <c r="G58" t="n">
-        <v>0.309</v>
+        <v>0.279</v>
       </c>
     </row>
     <row r="59">
@@ -1897,22 +1897,22 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.043</v>
+        <v>-0.167</v>
       </c>
       <c r="C59" t="n">
-        <v>1.478</v>
+        <v>1.584</v>
       </c>
       <c r="D59" t="n">
-        <v>0.467</v>
+        <v>0.569</v>
       </c>
       <c r="E59" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.754</v>
       </c>
       <c r="F59" t="n">
-        <v>0.738</v>
+        <v>0.708</v>
       </c>
       <c r="G59" t="n">
-        <v>0.405</v>
+        <v>0.226</v>
       </c>
     </row>
     <row r="60">
@@ -1922,22 +1922,22 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.136</v>
+        <v>0.31</v>
       </c>
       <c r="C60" t="n">
-        <v>3.592</v>
+        <v>3.07</v>
       </c>
       <c r="D60" t="n">
-        <v>0.422</v>
+        <v>0.337</v>
       </c>
       <c r="E60" t="n">
-        <v>0.65</v>
+        <v>0.581</v>
       </c>
       <c r="F60" t="n">
-        <v>0.784</v>
+        <v>0.733</v>
       </c>
       <c r="G60" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.623</v>
       </c>
     </row>
     <row r="61">
@@ -1947,22 +1947,22 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>-0.074</v>
+        <v>0.01</v>
       </c>
       <c r="C61" t="n">
-        <v>1.537</v>
+        <v>1.495</v>
       </c>
       <c r="D61" t="n">
-        <v>0.524</v>
+        <v>0.483</v>
       </c>
       <c r="E61" t="n">
-        <v>0.724</v>
+        <v>0.695</v>
       </c>
       <c r="F61" t="n">
-        <v>0.6870000000000001</v>
+        <v>0.6840000000000001</v>
       </c>
       <c r="G61" t="n">
-        <v>0.231</v>
+        <v>0.294</v>
       </c>
     </row>
     <row r="62">
@@ -1997,22 +1997,22 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.304</v>
+        <v>0.296</v>
       </c>
       <c r="C63" t="n">
-        <v>1.348</v>
+        <v>1.352</v>
       </c>
       <c r="D63" t="n">
-        <v>0.348</v>
+        <v>0.352</v>
       </c>
       <c r="E63" t="n">
-        <v>0.59</v>
+        <v>0.593</v>
       </c>
       <c r="F63" t="n">
-        <v>0.733</v>
+        <v>0.713</v>
       </c>
       <c r="G63" t="n">
-        <v>0.6919999999999999</v>
+        <v>0.653</v>
       </c>
     </row>
     <row r="64">
@@ -2022,22 +2022,22 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.253</v>
+        <v>0.32</v>
       </c>
       <c r="C64" t="n">
-        <v>1.374</v>
+        <v>1.34</v>
       </c>
       <c r="D64" t="n">
-        <v>0.373</v>
+        <v>0.34</v>
       </c>
       <c r="E64" t="n">
-        <v>0.611</v>
+        <v>0.583</v>
       </c>
       <c r="F64" t="n">
         <v>0.609</v>
       </c>
       <c r="G64" t="n">
-        <v>0.593</v>
+        <v>0.645</v>
       </c>
     </row>
     <row r="65">
@@ -2047,22 +2047,22 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.176</v>
+        <v>-0.183</v>
       </c>
       <c r="C65" t="n">
-        <v>3.472</v>
+        <v>4.549</v>
       </c>
       <c r="D65" t="n">
-        <v>0.412</v>
+        <v>0.592</v>
       </c>
       <c r="E65" t="n">
-        <v>0.642</v>
+        <v>0.769</v>
       </c>
       <c r="F65" t="n">
-        <v>0.59</v>
+        <v>0.587</v>
       </c>
       <c r="G65" t="n">
-        <v>0.441</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="66">
@@ -2072,22 +2072,22 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.286</v>
+        <v>0.35</v>
       </c>
       <c r="C66" t="n">
-        <v>1.357</v>
+        <v>1.325</v>
       </c>
       <c r="D66" t="n">
-        <v>0.357</v>
+        <v>0.325</v>
       </c>
       <c r="E66" t="n">
-        <v>0.597</v>
+        <v>0.57</v>
       </c>
       <c r="F66" t="n">
-        <v>0.6929999999999999</v>
+        <v>0.678</v>
       </c>
       <c r="G66" t="n">
-        <v>0.601</v>
+        <v>0.652</v>
       </c>
     </row>
     <row r="67">
@@ -2122,22 +2122,22 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.661</v>
+        <v>0.734</v>
       </c>
       <c r="C68" t="n">
-        <v>1.17</v>
+        <v>1.133</v>
       </c>
       <c r="D68" t="n">
-        <v>0.134</v>
+        <v>0.105</v>
       </c>
       <c r="E68" t="n">
-        <v>0.366</v>
+        <v>0.324</v>
       </c>
       <c r="F68" t="n">
-        <v>0.654</v>
+        <v>0.645</v>
       </c>
       <c r="G68" t="n">
-        <v>0.821</v>
+        <v>0.867</v>
       </c>
     </row>
     <row r="69">
@@ -2147,22 +2147,22 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.17</v>
+        <v>0.53</v>
       </c>
       <c r="C69" t="n">
-        <v>1.415</v>
+        <v>1.235</v>
       </c>
       <c r="D69" t="n">
-        <v>0.326</v>
+        <v>0.185</v>
       </c>
       <c r="E69" t="n">
-        <v>0.571</v>
+        <v>0.43</v>
       </c>
       <c r="F69" t="n">
-        <v>0.59</v>
+        <v>0.596</v>
       </c>
       <c r="G69" t="n">
-        <v>0.461</v>
+        <v>0.742</v>
       </c>
     </row>
     <row r="70">
@@ -2172,22 +2172,22 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.514</v>
+        <v>0.239</v>
       </c>
       <c r="C70" t="n">
-        <v>2.458</v>
+        <v>3.283</v>
       </c>
       <c r="D70" t="n">
-        <v>0.191</v>
+        <v>0.3</v>
       </c>
       <c r="E70" t="n">
-        <v>0.437</v>
+        <v>0.548</v>
       </c>
       <c r="F70" t="n">
-        <v>0.578</v>
+        <v>0.587</v>
       </c>
       <c r="G70" t="n">
-        <v>0.753</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="71">
@@ -2197,97 +2197,97 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.65</v>
+        <v>0.624</v>
       </c>
       <c r="C71" t="n">
-        <v>1.175</v>
+        <v>1.188</v>
       </c>
       <c r="D71" t="n">
-        <v>0.138</v>
+        <v>0.148</v>
       </c>
       <c r="E71" t="n">
-        <v>0.371</v>
+        <v>0.385</v>
       </c>
       <c r="F71" t="n">
-        <v>0.595</v>
+        <v>0.598</v>
       </c>
       <c r="G71" t="n">
-        <v>0.837</v>
+        <v>0.832</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="inlineStr">
         <is>
-          <t>LR340</t>
+          <t>LR335</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>-0.169</v>
+        <v>-0.67</v>
       </c>
       <c r="C72" t="n">
-        <v>1.584</v>
+        <v>1.29</v>
       </c>
       <c r="D72" t="n">
-        <v>1.195</v>
+        <v>0.181</v>
       </c>
       <c r="E72" t="n">
-        <v>1.093</v>
+        <v>0.425</v>
       </c>
       <c r="F72" t="n">
-        <v>1.46</v>
+        <v>0.45</v>
       </c>
       <c r="G72" t="n">
-        <v>0.711</v>
+        <v>0.486</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="inlineStr">
         <is>
-          <t>RF340</t>
+          <t>RF335</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.036</v>
+        <v>0.535</v>
       </c>
       <c r="C73" t="n">
-        <v>1.482</v>
+        <v>1.081</v>
       </c>
       <c r="D73" t="n">
-        <v>0.985</v>
+        <v>0.05</v>
       </c>
       <c r="E73" t="n">
-        <v>0.992</v>
+        <v>0.224</v>
       </c>
       <c r="F73" t="n">
-        <v>0.981</v>
+        <v>0.393</v>
       </c>
       <c r="G73" t="n">
-        <v>0.423</v>
+        <v>0.946</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="inlineStr">
         <is>
-          <t>NN340</t>
+          <t>NN335</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>-1.969</v>
+        <v>-0.424</v>
       </c>
       <c r="C74" t="n">
-        <v>2.484</v>
+        <v>1.248</v>
       </c>
       <c r="D74" t="n">
-        <v>3.036</v>
+        <v>0.154</v>
       </c>
       <c r="E74" t="n">
-        <v>1.742</v>
+        <v>0.392</v>
       </c>
       <c r="F74" t="n">
-        <v>1.207</v>
+        <v>0.395</v>
       </c>
       <c r="G74" t="n">
-        <v>-0.318</v>
+        <v>0.417</v>
       </c>
     </row>
     <row r="75">
@@ -2297,22 +2297,22 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>-12.306</v>
+        <v>-2.909</v>
       </c>
       <c r="C75" t="n">
-        <v>40.918</v>
+        <v>2.954</v>
       </c>
       <c r="D75" t="n">
-        <v>13.608</v>
+        <v>0.424</v>
       </c>
       <c r="E75" t="n">
-        <v>3.689</v>
+        <v>0.651</v>
       </c>
       <c r="F75" t="n">
-        <v>1.944</v>
+        <v>0.447</v>
       </c>
       <c r="G75" t="n">
-        <v>0.08400000000000001</v>
+        <v>-0.919</v>
       </c>
     </row>
     <row r="76">
@@ -2322,97 +2322,97 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.538</v>
+        <v>-0.313</v>
       </c>
       <c r="C76" t="n">
-        <v>1.231</v>
+        <v>1.228</v>
       </c>
       <c r="D76" t="n">
-        <v>0.473</v>
+        <v>0.142</v>
       </c>
       <c r="E76" t="n">
-        <v>0.6879999999999999</v>
+        <v>0.377</v>
       </c>
       <c r="F76" t="n">
-        <v>1.088</v>
+        <v>0.4</v>
       </c>
       <c r="G76" t="n">
-        <v>0.772</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="inlineStr">
         <is>
-          <t>LR342</t>
+          <t>LR346</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>-18099679.146</v>
+        <v>-187.133</v>
       </c>
       <c r="C77" t="n">
-        <v>696142.544</v>
+        <v>8.236000000000001</v>
       </c>
       <c r="D77" t="n">
-        <v>7716784.443</v>
+        <v>14.308</v>
       </c>
       <c r="E77" t="n">
-        <v>2777.91</v>
+        <v>3.783</v>
       </c>
       <c r="F77" t="n">
-        <v>2017.931</v>
+        <v>3.774</v>
       </c>
       <c r="G77" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="inlineStr">
         <is>
-          <t>RF342</t>
+          <t>RF346</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>-4.759</v>
+        <v>-1.481</v>
       </c>
       <c r="C78" t="n">
-        <v>1.222</v>
+        <v>1.095</v>
       </c>
       <c r="D78" t="n">
-        <v>2.455</v>
+        <v>0.189</v>
       </c>
       <c r="E78" t="n">
-        <v>1.567</v>
+        <v>0.435</v>
       </c>
       <c r="F78" t="n">
-        <v>1.563</v>
+        <v>0.295</v>
       </c>
       <c r="G78" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="inlineStr">
         <is>
-          <t>NN342</t>
+          <t>NN346</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>-14.295</v>
+        <v>-14.7</v>
       </c>
       <c r="C79" t="n">
-        <v>1.588</v>
+        <v>1.604</v>
       </c>
       <c r="D79" t="n">
-        <v>6.521</v>
+        <v>1.194</v>
       </c>
       <c r="E79" t="n">
-        <v>2.554</v>
+        <v>1.093</v>
       </c>
       <c r="F79" t="n">
-        <v>2.403</v>
+        <v>1.02</v>
       </c>
       <c r="G79" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
@@ -2422,22 +2422,22 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>-6.659</v>
+        <v>-39.245</v>
       </c>
       <c r="C80" t="n">
-        <v>1.696</v>
+        <v>4.659</v>
       </c>
       <c r="D80" t="n">
-        <v>3.265</v>
+        <v>3.061</v>
       </c>
       <c r="E80" t="n">
-        <v>1.807</v>
+        <v>1.75</v>
       </c>
       <c r="F80" t="n">
-        <v>1.77</v>
+        <v>1.449</v>
       </c>
       <c r="G80" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="81">
@@ -2447,44 +2447,44 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>-2012651.233</v>
+        <v>-12.584</v>
       </c>
       <c r="C81" t="n">
-        <v>77410.701</v>
+        <v>1.522</v>
       </c>
       <c r="D81" t="n">
-        <v>858092.702</v>
+        <v>1.033</v>
       </c>
       <c r="E81" t="n">
-        <v>926.333</v>
+        <v>1.016</v>
       </c>
       <c r="F81" t="n">
-        <v>673.208</v>
+        <v>0.992</v>
       </c>
       <c r="G81" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="inlineStr">
         <is>
-          <t>LR344</t>
+          <t>LR348</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>-15284324.073</v>
+        <v>-251350.571</v>
       </c>
       <c r="C82" t="n">
-        <v>587859.657</v>
+        <v>9668.368</v>
       </c>
       <c r="D82" t="n">
-        <v>9522756.773</v>
+        <v>5036.255</v>
       </c>
       <c r="E82" t="n">
-        <v>3085.896</v>
+        <v>70.967</v>
       </c>
       <c r="F82" t="n">
-        <v>2725.555</v>
+        <v>60.412</v>
       </c>
       <c r="G82" t="n">
         <v>-1</v>
@@ -2493,23 +2493,23 @@
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>RF344</t>
+          <t>RF348</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>-1.848</v>
+        <v>-9.105</v>
       </c>
       <c r="C83" t="n">
-        <v>1.11</v>
+        <v>1.389</v>
       </c>
       <c r="D83" t="n">
-        <v>1.775</v>
+        <v>0.202</v>
       </c>
       <c r="E83" t="n">
-        <v>1.332</v>
+        <v>0.449</v>
       </c>
       <c r="F83" t="n">
-        <v>1.655</v>
+        <v>0.511</v>
       </c>
       <c r="G83" t="n">
         <v>1</v>
@@ -2518,23 +2518,23 @@
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>NN344</t>
+          <t>NN348</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>-12.197</v>
+        <v>-1.229</v>
       </c>
       <c r="C84" t="n">
-        <v>1.508</v>
+        <v>1.086</v>
       </c>
       <c r="D84" t="n">
-        <v>8.223000000000001</v>
+        <v>0.045</v>
       </c>
       <c r="E84" t="n">
-        <v>2.868</v>
+        <v>0.212</v>
       </c>
       <c r="F84" t="n">
-        <v>2.841</v>
+        <v>0.272</v>
       </c>
       <c r="G84" t="n">
         <v>1</v>
@@ -2547,19 +2547,19 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>-114.507</v>
+        <v>-80.925</v>
       </c>
       <c r="C85" t="n">
-        <v>11.501</v>
+        <v>8.448</v>
       </c>
       <c r="D85" t="n">
-        <v>71.96599999999999</v>
+        <v>1.642</v>
       </c>
       <c r="E85" t="n">
-        <v>8.483000000000001</v>
+        <v>1.281</v>
       </c>
       <c r="F85" t="n">
-        <v>7.199</v>
+        <v>1.041</v>
       </c>
       <c r="G85" t="n">
         <v>1</v>
@@ -2572,19 +2572,19 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>-1699263.789</v>
+        <v>-28276.771</v>
       </c>
       <c r="C86" t="n">
-        <v>65357.338</v>
+        <v>1088.607</v>
       </c>
       <c r="D86" t="n">
-        <v>1058711.144</v>
+        <v>566.593</v>
       </c>
       <c r="E86" t="n">
-        <v>1028.937</v>
+        <v>23.803</v>
       </c>
       <c r="F86" t="n">
-        <v>909.255</v>
+        <v>20.373</v>
       </c>
       <c r="G86" t="n">
         <v>-1</v>
@@ -2593,23 +2593,23 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>LR346</t>
+          <t>LR350</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>-187.133</v>
+        <v>-880.062</v>
       </c>
       <c r="C87" t="n">
-        <v>8.236000000000001</v>
+        <v>34.887</v>
       </c>
       <c r="D87" t="n">
-        <v>14.308</v>
+        <v>44.48</v>
       </c>
       <c r="E87" t="n">
-        <v>3.783</v>
+        <v>6.669</v>
       </c>
       <c r="F87" t="n">
-        <v>3.774</v>
+        <v>5.849</v>
       </c>
       <c r="G87" t="n">
         <v>1</v>
@@ -2618,48 +2618,48 @@
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>RF346</t>
+          <t>RF350</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>-0.696</v>
+        <v>-3.17</v>
       </c>
       <c r="C88" t="n">
-        <v>1.065</v>
+        <v>1.16</v>
       </c>
       <c r="D88" t="n">
-        <v>0.129</v>
+        <v>0.211</v>
       </c>
       <c r="E88" t="n">
-        <v>0.359</v>
+        <v>0.459</v>
       </c>
       <c r="F88" t="n">
-        <v>0.276</v>
+        <v>0.52</v>
       </c>
       <c r="G88" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>NN346</t>
+          <t>NN350</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>-17.786</v>
+        <v>-2.614</v>
       </c>
       <c r="C89" t="n">
-        <v>1.723</v>
+        <v>1.139</v>
       </c>
       <c r="D89" t="n">
-        <v>1.429</v>
+        <v>0.182</v>
       </c>
       <c r="E89" t="n">
-        <v>1.195</v>
+        <v>0.427</v>
       </c>
       <c r="F89" t="n">
-        <v>1.186</v>
+        <v>0.397</v>
       </c>
       <c r="G89" t="n">
         <v>1</v>
@@ -2672,19 +2672,19 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>-2.723</v>
+        <v>-3.58</v>
       </c>
       <c r="C90" t="n">
-        <v>1.338</v>
+        <v>1.416</v>
       </c>
       <c r="D90" t="n">
-        <v>0.283</v>
+        <v>0.231</v>
       </c>
       <c r="E90" t="n">
-        <v>0.532</v>
+        <v>0.481</v>
       </c>
       <c r="F90" t="n">
-        <v>0.649</v>
+        <v>0.479</v>
       </c>
       <c r="G90" t="n">
         <v>1</v>
@@ -2697,19 +2697,19 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>-23.441</v>
+        <v>-82.63</v>
       </c>
       <c r="C91" t="n">
-        <v>1.94</v>
+        <v>4.217</v>
       </c>
       <c r="D91" t="n">
-        <v>1.859</v>
+        <v>4.222</v>
       </c>
       <c r="E91" t="n">
-        <v>1.363</v>
+        <v>2.055</v>
       </c>
       <c r="F91" t="n">
-        <v>1.363</v>
+        <v>1.761</v>
       </c>
       <c r="G91" t="n">
         <v>1</v>
@@ -2718,48 +2718,48 @@
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>LR348</t>
+          <t>LR352</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>-251350.571</v>
+        <v>-1859.171</v>
       </c>
       <c r="C92" t="n">
-        <v>9668.368</v>
+        <v>72.545</v>
       </c>
       <c r="D92" t="n">
-        <v>5036.255</v>
+        <v>58.079</v>
       </c>
       <c r="E92" t="n">
-        <v>70.967</v>
+        <v>7.621</v>
       </c>
       <c r="F92" t="n">
-        <v>60.412</v>
+        <v>7.219</v>
       </c>
       <c r="G92" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>RF348</t>
+          <t>RF352</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>-14.313</v>
+        <v>-4.382</v>
       </c>
       <c r="C93" t="n">
-        <v>1.589</v>
+        <v>1.207</v>
       </c>
       <c r="D93" t="n">
-        <v>0.307</v>
+        <v>0.168</v>
       </c>
       <c r="E93" t="n">
-        <v>0.554</v>
+        <v>0.41</v>
       </c>
       <c r="F93" t="n">
-        <v>0.638</v>
+        <v>0.39</v>
       </c>
       <c r="G93" t="n">
         <v>1</v>
@@ -2768,23 +2768,23 @@
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>NN348</t>
+          <t>NN352</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>-12.861</v>
+        <v>-28.748</v>
       </c>
       <c r="C94" t="n">
-        <v>1.533</v>
+        <v>2.144</v>
       </c>
       <c r="D94" t="n">
-        <v>0.278</v>
+        <v>0.929</v>
       </c>
       <c r="E94" t="n">
-        <v>0.527</v>
+        <v>0.964</v>
       </c>
       <c r="F94" t="n">
-        <v>0.665</v>
+        <v>0.955</v>
       </c>
       <c r="G94" t="n">
         <v>1</v>
@@ -2797,22 +2797,22 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>-15.067</v>
+        <v>-8.616</v>
       </c>
       <c r="C95" t="n">
-        <v>2.461</v>
+        <v>1.874</v>
       </c>
       <c r="D95" t="n">
-        <v>0.322</v>
+        <v>0.3</v>
       </c>
       <c r="E95" t="n">
-        <v>0.5669999999999999</v>
+        <v>0.548</v>
       </c>
       <c r="F95" t="n">
-        <v>0.555</v>
+        <v>0.48</v>
       </c>
       <c r="G95" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="96">
@@ -2822,94 +2822,94 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>-28382.017</v>
+        <v>-173.487</v>
       </c>
       <c r="C96" t="n">
-        <v>1092.654</v>
+        <v>7.711</v>
       </c>
       <c r="D96" t="n">
-        <v>568.702</v>
+        <v>5.448</v>
       </c>
       <c r="E96" t="n">
-        <v>23.847</v>
+        <v>2.334</v>
       </c>
       <c r="F96" t="n">
-        <v>20.442</v>
+        <v>2.167</v>
       </c>
       <c r="G96" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>LR350</t>
+          <t>LR354</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>-880.062</v>
+        <v>-94.221</v>
       </c>
       <c r="C97" t="n">
-        <v>34.887</v>
+        <v>4.662</v>
       </c>
       <c r="D97" t="n">
-        <v>44.48</v>
+        <v>2.574</v>
       </c>
       <c r="E97" t="n">
-        <v>6.669</v>
+        <v>1.604</v>
       </c>
       <c r="F97" t="n">
-        <v>5.849</v>
+        <v>1.123</v>
       </c>
       <c r="G97" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>RF350</t>
+          <t>RF354</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>-3.659</v>
+        <v>-48.127</v>
       </c>
       <c r="C98" t="n">
-        <v>1.179</v>
+        <v>2.89</v>
       </c>
       <c r="D98" t="n">
-        <v>0.235</v>
+        <v>1.328</v>
       </c>
       <c r="E98" t="n">
-        <v>0.485</v>
+        <v>1.152</v>
       </c>
       <c r="F98" t="n">
-        <v>0.555</v>
+        <v>1.094</v>
       </c>
       <c r="G98" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>NN350</t>
+          <t>NN354</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>-42.184</v>
+        <v>-64.952</v>
       </c>
       <c r="C99" t="n">
-        <v>2.661</v>
+        <v>3.537</v>
       </c>
       <c r="D99" t="n">
-        <v>2.18</v>
+        <v>1.782</v>
       </c>
       <c r="E99" t="n">
-        <v>1.476</v>
+        <v>1.335</v>
       </c>
       <c r="F99" t="n">
-        <v>1.469</v>
+        <v>1.333</v>
       </c>
       <c r="G99" t="n">
         <v>1</v>
@@ -2922,19 +2922,19 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>-16.496</v>
+        <v>-74.175</v>
       </c>
       <c r="C100" t="n">
-        <v>2.591</v>
+        <v>7.834</v>
       </c>
       <c r="D100" t="n">
-        <v>0.883</v>
+        <v>2.032</v>
       </c>
       <c r="E100" t="n">
-        <v>0.9399999999999999</v>
+        <v>1.425</v>
       </c>
       <c r="F100" t="n">
-        <v>0.8159999999999999</v>
+        <v>1.174</v>
       </c>
       <c r="G100" t="n">
         <v>-1</v>
@@ -2947,69 +2947,69 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>-69.794</v>
+        <v>-49.839</v>
       </c>
       <c r="C101" t="n">
-        <v>3.723</v>
+        <v>2.955</v>
       </c>
       <c r="D101" t="n">
-        <v>3.574</v>
+        <v>1.374</v>
       </c>
       <c r="E101" t="n">
-        <v>1.891</v>
+        <v>1.172</v>
       </c>
       <c r="F101" t="n">
-        <v>1.549</v>
+        <v>1.008</v>
       </c>
       <c r="G101" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>LR352</t>
+          <t>LR356</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>-1859.171</v>
+        <v>-26.305</v>
       </c>
       <c r="C102" t="n">
-        <v>72.545</v>
+        <v>2.05</v>
       </c>
       <c r="D102" t="n">
-        <v>58.079</v>
+        <v>0.928</v>
       </c>
       <c r="E102" t="n">
-        <v>7.621</v>
+        <v>0.963</v>
       </c>
       <c r="F102" t="n">
-        <v>7.219</v>
+        <v>0.821</v>
       </c>
       <c r="G102" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>RF352</t>
+          <t>RF356</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>-7.489</v>
+        <v>-87.77200000000001</v>
       </c>
       <c r="C103" t="n">
-        <v>1.326</v>
+        <v>4.414</v>
       </c>
       <c r="D103" t="n">
-        <v>0.265</v>
+        <v>3.017</v>
       </c>
       <c r="E103" t="n">
-        <v>0.515</v>
+        <v>1.737</v>
       </c>
       <c r="F103" t="n">
-        <v>0.51</v>
+        <v>1.684</v>
       </c>
       <c r="G103" t="n">
         <v>1</v>
@@ -3018,26 +3018,26 @@
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>NN352</t>
+          <t>NN356</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>-23.288</v>
+        <v>-40.075</v>
       </c>
       <c r="C104" t="n">
-        <v>1.934</v>
+        <v>2.58</v>
       </c>
       <c r="D104" t="n">
-        <v>0.758</v>
+        <v>1.396</v>
       </c>
       <c r="E104" t="n">
-        <v>0.871</v>
+        <v>1.182</v>
       </c>
       <c r="F104" t="n">
-        <v>0.866</v>
+        <v>1.133</v>
       </c>
       <c r="G104" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="105">
@@ -3047,19 +3047,19 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>-8.936999999999999</v>
+        <v>-43.862</v>
       </c>
       <c r="C105" t="n">
-        <v>1.903</v>
+        <v>5.078</v>
       </c>
       <c r="D105" t="n">
-        <v>0.31</v>
+        <v>1.525</v>
       </c>
       <c r="E105" t="n">
-        <v>0.5570000000000001</v>
+        <v>1.235</v>
       </c>
       <c r="F105" t="n">
-        <v>0.728</v>
+        <v>1.057</v>
       </c>
       <c r="G105" t="n">
         <v>1</v>
@@ -3072,94 +3072,94 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>-104.547</v>
+        <v>-58.974</v>
       </c>
       <c r="C106" t="n">
-        <v>5.06</v>
+        <v>3.307</v>
       </c>
       <c r="D106" t="n">
-        <v>3.295</v>
+        <v>2.039</v>
       </c>
       <c r="E106" t="n">
-        <v>1.815</v>
+        <v>1.428</v>
       </c>
       <c r="F106" t="n">
-        <v>1.691</v>
+        <v>1.415</v>
       </c>
       <c r="G106" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>LR354</t>
+          <t>LR358</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>-94.221</v>
+        <v>-8.734999999999999</v>
       </c>
       <c r="C107" t="n">
-        <v>4.662</v>
+        <v>1.374</v>
       </c>
       <c r="D107" t="n">
-        <v>2.574</v>
+        <v>1.537</v>
       </c>
       <c r="E107" t="n">
-        <v>1.604</v>
+        <v>1.24</v>
       </c>
       <c r="F107" t="n">
-        <v>1.123</v>
+        <v>1.227</v>
       </c>
       <c r="G107" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>RF354</t>
+          <t>RF358</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>-52.394</v>
+        <v>-0.96</v>
       </c>
       <c r="C108" t="n">
-        <v>3.054</v>
+        <v>1.075</v>
       </c>
       <c r="D108" t="n">
-        <v>1.443</v>
+        <v>0.309</v>
       </c>
       <c r="E108" t="n">
-        <v>1.201</v>
+        <v>0.556</v>
       </c>
       <c r="F108" t="n">
-        <v>1.154</v>
+        <v>0.527</v>
       </c>
       <c r="G108" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>NN354</t>
+          <t>NN358</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>-37.857</v>
+        <v>-29.082</v>
       </c>
       <c r="C109" t="n">
-        <v>2.494</v>
+        <v>2.157</v>
       </c>
       <c r="D109" t="n">
-        <v>1.05</v>
+        <v>4.749</v>
       </c>
       <c r="E109" t="n">
-        <v>1.025</v>
+        <v>2.179</v>
       </c>
       <c r="F109" t="n">
-        <v>0.804</v>
+        <v>1.947</v>
       </c>
       <c r="G109" t="n">
         <v>-1</v>
@@ -3172,19 +3172,19 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>-80.002</v>
+        <v>-3.902</v>
       </c>
       <c r="C110" t="n">
-        <v>8.364000000000001</v>
+        <v>1.446</v>
       </c>
       <c r="D110" t="n">
-        <v>2.189</v>
+        <v>0.774</v>
       </c>
       <c r="E110" t="n">
-        <v>1.48</v>
+        <v>0.88</v>
       </c>
       <c r="F110" t="n">
-        <v>1.3</v>
+        <v>0.783</v>
       </c>
       <c r="G110" t="n">
         <v>-1</v>
@@ -3197,69 +3197,69 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>-58.18</v>
+        <v>-0.107</v>
       </c>
       <c r="C111" t="n">
-        <v>3.276</v>
+        <v>1.043</v>
       </c>
       <c r="D111" t="n">
-        <v>1.599</v>
+        <v>0.175</v>
       </c>
       <c r="E111" t="n">
-        <v>1.265</v>
+        <v>0.418</v>
       </c>
       <c r="F111" t="n">
-        <v>1.131</v>
+        <v>0.629</v>
       </c>
       <c r="G111" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>LR356</t>
+          <t>LR360</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>-26.305</v>
+        <v>-1.157</v>
       </c>
       <c r="C112" t="n">
-        <v>2.05</v>
+        <v>1.083</v>
       </c>
       <c r="D112" t="n">
-        <v>0.928</v>
+        <v>1.413</v>
       </c>
       <c r="E112" t="n">
-        <v>0.963</v>
+        <v>1.189</v>
       </c>
       <c r="F112" t="n">
-        <v>0.821</v>
+        <v>1.227</v>
       </c>
       <c r="G112" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>RF356</t>
+          <t>RF360</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>-99.84699999999999</v>
+        <v>-1.002</v>
       </c>
       <c r="C113" t="n">
-        <v>4.879</v>
+        <v>1.077</v>
       </c>
       <c r="D113" t="n">
-        <v>3.428</v>
+        <v>1.312</v>
       </c>
       <c r="E113" t="n">
-        <v>1.851</v>
+        <v>1.145</v>
       </c>
       <c r="F113" t="n">
-        <v>1.79</v>
+        <v>1.33</v>
       </c>
       <c r="G113" t="n">
         <v>1</v>
@@ -3268,26 +3268,26 @@
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>NN356</t>
+          <t>NN360</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>-24.664</v>
+        <v>-4.245</v>
       </c>
       <c r="C114" t="n">
-        <v>1.987</v>
+        <v>1.202</v>
       </c>
       <c r="D114" t="n">
-        <v>0.872</v>
+        <v>3.438</v>
       </c>
       <c r="E114" t="n">
-        <v>0.9340000000000001</v>
+        <v>1.854</v>
       </c>
       <c r="F114" t="n">
-        <v>0.9330000000000001</v>
+        <v>1.566</v>
       </c>
       <c r="G114" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="115">
@@ -3297,22 +3297,22 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>-27.676</v>
+        <v>0.819</v>
       </c>
       <c r="C115" t="n">
-        <v>3.607</v>
+        <v>1.016</v>
       </c>
       <c r="D115" t="n">
-        <v>0.975</v>
+        <v>0.118</v>
       </c>
       <c r="E115" t="n">
-        <v>0.987</v>
+        <v>0.344</v>
       </c>
       <c r="F115" t="n">
-        <v>0.698</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="G115" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -3322,19 +3322,19 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>-63.127</v>
+        <v>-1.167</v>
       </c>
       <c r="C116" t="n">
-        <v>3.466</v>
+        <v>1.083</v>
       </c>
       <c r="D116" t="n">
-        <v>2.18</v>
+        <v>1.42</v>
       </c>
       <c r="E116" t="n">
-        <v>1.476</v>
+        <v>1.192</v>
       </c>
       <c r="F116" t="n">
-        <v>1.476</v>
+        <v>1.109</v>
       </c>
       <c r="G116" t="n">
         <v>1</v>
@@ -3343,48 +3343,48 @@
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>LR358</t>
+          <t>LR362</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>-8.734999999999999</v>
+        <v>-32.886</v>
       </c>
       <c r="C117" t="n">
-        <v>1.374</v>
+        <v>2.303</v>
       </c>
       <c r="D117" t="n">
-        <v>1.537</v>
+        <v>2.407</v>
       </c>
       <c r="E117" t="n">
-        <v>1.24</v>
+        <v>1.551</v>
       </c>
       <c r="F117" t="n">
-        <v>1.227</v>
+        <v>1.488</v>
       </c>
       <c r="G117" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>RF358</t>
+          <t>RF362</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>-1.164</v>
+        <v>-5.419</v>
       </c>
       <c r="C118" t="n">
-        <v>1.083</v>
+        <v>1.247</v>
       </c>
       <c r="D118" t="n">
-        <v>0.342</v>
+        <v>0.456</v>
       </c>
       <c r="E118" t="n">
-        <v>0.585</v>
+        <v>0.675</v>
       </c>
       <c r="F118" t="n">
-        <v>0.613</v>
+        <v>0.644</v>
       </c>
       <c r="G118" t="n">
         <v>1</v>
@@ -3393,26 +3393,26 @@
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>NN358</t>
+          <t>NN362</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>-9.201000000000001</v>
+        <v>-8.956</v>
       </c>
       <c r="C119" t="n">
-        <v>1.392</v>
+        <v>1.383</v>
       </c>
       <c r="D119" t="n">
-        <v>1.61</v>
+        <v>0.707</v>
       </c>
       <c r="E119" t="n">
-        <v>1.269</v>
+        <v>0.841</v>
       </c>
       <c r="F119" t="n">
-        <v>1.096</v>
+        <v>0.838</v>
       </c>
       <c r="G119" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
@@ -3422,22 +3422,22 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>-0.264</v>
+        <v>-26.624</v>
       </c>
       <c r="C120" t="n">
-        <v>1.115</v>
+        <v>3.511</v>
       </c>
       <c r="D120" t="n">
-        <v>0.2</v>
+        <v>1.962</v>
       </c>
       <c r="E120" t="n">
-        <v>0.447</v>
+        <v>1.401</v>
       </c>
       <c r="F120" t="n">
-        <v>0.426</v>
+        <v>1.325</v>
       </c>
       <c r="G120" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="121">
@@ -3447,44 +3447,44 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>-1.613</v>
+        <v>-4.901</v>
       </c>
       <c r="C121" t="n">
-        <v>1.1</v>
+        <v>1.227</v>
       </c>
       <c r="D121" t="n">
-        <v>0.412</v>
+        <v>0.419</v>
       </c>
       <c r="E121" t="n">
-        <v>0.642</v>
+        <v>0.647</v>
       </c>
       <c r="F121" t="n">
-        <v>0.756</v>
+        <v>0.59</v>
       </c>
       <c r="G121" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>LR360</t>
+          <t>LR364</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>-1.157</v>
+        <v>-6487.321</v>
       </c>
       <c r="C122" t="n">
-        <v>1.083</v>
+        <v>250.551</v>
       </c>
       <c r="D122" t="n">
-        <v>1.413</v>
+        <v>70.372</v>
       </c>
       <c r="E122" t="n">
-        <v>1.189</v>
+        <v>8.388999999999999</v>
       </c>
       <c r="F122" t="n">
-        <v>1.227</v>
+        <v>7.098</v>
       </c>
       <c r="G122" t="n">
         <v>1</v>
@@ -3493,23 +3493,23 @@
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>RF360</t>
+          <t>RF364</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>-0.88</v>
+        <v>-292.405</v>
       </c>
       <c r="C123" t="n">
-        <v>1.072</v>
+        <v>12.285</v>
       </c>
       <c r="D123" t="n">
-        <v>1.232</v>
+        <v>3.182</v>
       </c>
       <c r="E123" t="n">
-        <v>1.11</v>
+        <v>1.784</v>
       </c>
       <c r="F123" t="n">
-        <v>1.164</v>
+        <v>1.73</v>
       </c>
       <c r="G123" t="n">
         <v>1</v>
@@ -3518,23 +3518,23 @@
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>NN360</t>
+          <t>NN364</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>-11.775</v>
+        <v>-238.34</v>
       </c>
       <c r="C124" t="n">
-        <v>1.491</v>
+        <v>10.205</v>
       </c>
       <c r="D124" t="n">
-        <v>8.372</v>
+        <v>2.596</v>
       </c>
       <c r="E124" t="n">
-        <v>2.893</v>
+        <v>1.611</v>
       </c>
       <c r="F124" t="n">
-        <v>2.82</v>
+        <v>1.6</v>
       </c>
       <c r="G124" t="n">
         <v>1</v>
@@ -3547,19 +3547,19 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>-0.78</v>
+        <v>-5571.649</v>
       </c>
       <c r="C125" t="n">
-        <v>1.162</v>
+        <v>507.604</v>
       </c>
       <c r="D125" t="n">
-        <v>1.167</v>
+        <v>60.44</v>
       </c>
       <c r="E125" t="n">
-        <v>1.08</v>
+        <v>7.774</v>
       </c>
       <c r="F125" t="n">
-        <v>1.323</v>
+        <v>6.534</v>
       </c>
       <c r="G125" t="n">
         <v>1</v>
@@ -3572,19 +3572,19 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>-0.963</v>
+        <v>-1475.344</v>
       </c>
       <c r="C126" t="n">
-        <v>1.076</v>
+        <v>57.782</v>
       </c>
       <c r="D126" t="n">
-        <v>1.286</v>
+        <v>16.012</v>
       </c>
       <c r="E126" t="n">
-        <v>1.134</v>
+        <v>4.001</v>
       </c>
       <c r="F126" t="n">
-        <v>1.036</v>
+        <v>3.71</v>
       </c>
       <c r="G126" t="n">
         <v>1</v>
@@ -3593,48 +3593,48 @@
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>LR362</t>
+          <t>LR366</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>-32.886</v>
+        <v>0.139</v>
       </c>
       <c r="C127" t="n">
-        <v>2.303</v>
+        <v>1.033</v>
       </c>
       <c r="D127" t="n">
-        <v>2.407</v>
+        <v>1.089</v>
       </c>
       <c r="E127" t="n">
-        <v>1.551</v>
+        <v>1.044</v>
       </c>
       <c r="F127" t="n">
-        <v>1.488</v>
+        <v>1.125</v>
       </c>
       <c r="G127" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>RF362</t>
+          <t>RF366</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>-2.951</v>
+        <v>-1.031</v>
       </c>
       <c r="C128" t="n">
-        <v>1.152</v>
+        <v>1.078</v>
       </c>
       <c r="D128" t="n">
-        <v>0.281</v>
+        <v>2.568</v>
       </c>
       <c r="E128" t="n">
-        <v>0.53</v>
+        <v>1.602</v>
       </c>
       <c r="F128" t="n">
-        <v>0.54</v>
+        <v>1.153</v>
       </c>
       <c r="G128" t="n">
         <v>1</v>
@@ -3643,26 +3643,26 @@
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>NN362</t>
+          <t>NN366</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>-20.002</v>
+        <v>-0.611</v>
       </c>
       <c r="C129" t="n">
-        <v>1.808</v>
+        <v>1.062</v>
       </c>
       <c r="D129" t="n">
-        <v>1.492</v>
+        <v>2.037</v>
       </c>
       <c r="E129" t="n">
-        <v>1.221</v>
+        <v>1.427</v>
       </c>
       <c r="F129" t="n">
-        <v>1.095</v>
+        <v>1.125</v>
       </c>
       <c r="G129" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="130">
@@ -3672,22 +3672,22 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>-9.103</v>
+        <v>-0.43</v>
       </c>
       <c r="C130" t="n">
-        <v>1.918</v>
+        <v>1.13</v>
       </c>
       <c r="D130" t="n">
-        <v>0.718</v>
+        <v>1.809</v>
       </c>
       <c r="E130" t="n">
-        <v>0.847</v>
+        <v>1.345</v>
       </c>
       <c r="F130" t="n">
-        <v>0.8149999999999999</v>
+        <v>1.125</v>
       </c>
       <c r="G130" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="131">
@@ -3697,19 +3697,19 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>-2.432</v>
+        <v>-0.695</v>
       </c>
       <c r="C131" t="n">
-        <v>1.132</v>
+        <v>1.065</v>
       </c>
       <c r="D131" t="n">
-        <v>0.244</v>
+        <v>2.144</v>
       </c>
       <c r="E131" t="n">
-        <v>0.494</v>
+        <v>1.464</v>
       </c>
       <c r="F131" t="n">
-        <v>0.426</v>
+        <v>1.125</v>
       </c>
       <c r="G131" t="n">
         <v>1</v>
@@ -3718,23 +3718,23 @@
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>LR364</t>
+          <t>LR368</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>-6487.321</v>
+        <v>-580.784</v>
       </c>
       <c r="C132" t="n">
-        <v>250.551</v>
+        <v>23.376</v>
       </c>
       <c r="D132" t="n">
-        <v>70.372</v>
+        <v>89.709</v>
       </c>
       <c r="E132" t="n">
-        <v>8.388999999999999</v>
+        <v>9.471</v>
       </c>
       <c r="F132" t="n">
-        <v>7.098</v>
+        <v>9.468999999999999</v>
       </c>
       <c r="G132" t="n">
         <v>1</v>
@@ -3743,23 +3743,23 @@
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>RF364</t>
+          <t>RF368</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>-270.672</v>
+        <v>-32.813</v>
       </c>
       <c r="C133" t="n">
-        <v>11.449</v>
+        <v>2.3</v>
       </c>
       <c r="D133" t="n">
-        <v>2.947</v>
+        <v>5.214</v>
       </c>
       <c r="E133" t="n">
-        <v>1.717</v>
+        <v>2.283</v>
       </c>
       <c r="F133" t="n">
-        <v>1.706</v>
+        <v>2.257</v>
       </c>
       <c r="G133" t="n">
         <v>1</v>
@@ -3768,23 +3768,23 @@
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>NN364</t>
+          <t>NN368</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>-647.9400000000001</v>
+        <v>-24.295</v>
       </c>
       <c r="C134" t="n">
-        <v>25.959</v>
+        <v>1.973</v>
       </c>
       <c r="D134" t="n">
-        <v>7.038</v>
+        <v>3.9</v>
       </c>
       <c r="E134" t="n">
-        <v>2.653</v>
+        <v>1.975</v>
       </c>
       <c r="F134" t="n">
-        <v>1.979</v>
+        <v>1.973</v>
       </c>
       <c r="G134" t="n">
         <v>1</v>
@@ -3797,22 +3797,22 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>-965.818</v>
+        <v>-63.948</v>
       </c>
       <c r="C135" t="n">
-        <v>88.893</v>
+        <v>6.904</v>
       </c>
       <c r="D135" t="n">
-        <v>10.486</v>
+        <v>10.015</v>
       </c>
       <c r="E135" t="n">
-        <v>3.238</v>
+        <v>3.165</v>
       </c>
       <c r="F135" t="n">
-        <v>2.7</v>
+        <v>2.894</v>
       </c>
       <c r="G135" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="136">
@@ -3822,19 +3822,19 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>-1341.815</v>
+        <v>-20.139</v>
       </c>
       <c r="C136" t="n">
-        <v>52.647</v>
+        <v>1.813</v>
       </c>
       <c r="D136" t="n">
-        <v>14.564</v>
+        <v>3.26</v>
       </c>
       <c r="E136" t="n">
-        <v>3.816</v>
+        <v>1.806</v>
       </c>
       <c r="F136" t="n">
-        <v>3.4</v>
+        <v>1.805</v>
       </c>
       <c r="G136" t="n">
         <v>1</v>
@@ -3843,23 +3843,23 @@
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>LR366</t>
+          <t>LR370</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.139</v>
+        <v>-2829.58</v>
       </c>
       <c r="C137" t="n">
-        <v>1.033</v>
+        <v>109.868</v>
       </c>
       <c r="D137" t="n">
-        <v>1.089</v>
+        <v>3.312</v>
       </c>
       <c r="E137" t="n">
-        <v>1.044</v>
+        <v>1.82</v>
       </c>
       <c r="F137" t="n">
-        <v>1.125</v>
+        <v>1.56</v>
       </c>
       <c r="G137" t="n">
         <v>1</v>
@@ -3868,23 +3868,23 @@
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>RF366</t>
+          <t>RF370</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>-0.802</v>
+        <v>-3569.942</v>
       </c>
       <c r="C138" t="n">
-        <v>1.069</v>
+        <v>138.344</v>
       </c>
       <c r="D138" t="n">
-        <v>2.279</v>
+        <v>4.178</v>
       </c>
       <c r="E138" t="n">
-        <v>1.51</v>
+        <v>2.044</v>
       </c>
       <c r="F138" t="n">
-        <v>1.191</v>
+        <v>1.563</v>
       </c>
       <c r="G138" t="n">
         <v>1</v>
@@ -3893,26 +3893,26 @@
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>NN366</t>
+          <t>NN370</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>-0.47</v>
+        <v>-14107.117</v>
       </c>
       <c r="C139" t="n">
-        <v>1.057</v>
+        <v>543.62</v>
       </c>
       <c r="D139" t="n">
-        <v>1.86</v>
+        <v>16.506</v>
       </c>
       <c r="E139" t="n">
-        <v>1.364</v>
+        <v>4.063</v>
       </c>
       <c r="F139" t="n">
-        <v>1.125</v>
+        <v>3.912</v>
       </c>
       <c r="G139" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140">
@@ -3922,19 +3922,19 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>0.821</v>
+        <v>-221.249</v>
       </c>
       <c r="C140" t="n">
-        <v>1.016</v>
+        <v>21.204</v>
       </c>
       <c r="D140" t="n">
-        <v>0.227</v>
+        <v>0.26</v>
       </c>
       <c r="E140" t="n">
-        <v>0.476</v>
+        <v>0.51</v>
       </c>
       <c r="F140" t="n">
-        <v>1.461</v>
+        <v>0.45</v>
       </c>
       <c r="G140" t="n">
         <v>1</v>
@@ -3947,19 +3947,19 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>-0.8169999999999999</v>
+        <v>-3707.383</v>
       </c>
       <c r="C141" t="n">
-        <v>1.07</v>
+        <v>143.63</v>
       </c>
       <c r="D141" t="n">
-        <v>2.299</v>
+        <v>4.339</v>
       </c>
       <c r="E141" t="n">
-        <v>1.516</v>
+        <v>2.083</v>
       </c>
       <c r="F141" t="n">
-        <v>1.199</v>
+        <v>1.748</v>
       </c>
       <c r="G141" t="n">
         <v>1</v>
@@ -3968,48 +3968,48 @@
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>LR368</t>
+          <t>LR372</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>-580.784</v>
+        <v>-4.334</v>
       </c>
       <c r="C142" t="n">
-        <v>23.376</v>
+        <v>1.205</v>
       </c>
       <c r="D142" t="n">
-        <v>89.709</v>
+        <v>0.406</v>
       </c>
       <c r="E142" t="n">
-        <v>9.471</v>
+        <v>0.637</v>
       </c>
       <c r="F142" t="n">
-        <v>9.468999999999999</v>
+        <v>0.573</v>
       </c>
       <c r="G142" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>RF368</t>
+          <t>RF372</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>-24.15</v>
+        <v>-5.334</v>
       </c>
       <c r="C143" t="n">
-        <v>1.967</v>
+        <v>1.244</v>
       </c>
       <c r="D143" t="n">
-        <v>3.878</v>
+        <v>0.482</v>
       </c>
       <c r="E143" t="n">
-        <v>1.969</v>
+        <v>0.694</v>
       </c>
       <c r="F143" t="n">
-        <v>1.963</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="G143" t="n">
         <v>1</v>
@@ -4018,23 +4018,23 @@
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>NN368</t>
+          <t>NN372</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>-52.262</v>
+        <v>-13.199</v>
       </c>
       <c r="C144" t="n">
-        <v>3.049</v>
+        <v>1.546</v>
       </c>
       <c r="D144" t="n">
-        <v>8.212999999999999</v>
+        <v>1.081</v>
       </c>
       <c r="E144" t="n">
-        <v>2.866</v>
+        <v>1.04</v>
       </c>
       <c r="F144" t="n">
-        <v>2.844</v>
+        <v>1.03</v>
       </c>
       <c r="G144" t="n">
         <v>1</v>
@@ -4047,19 +4047,19 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>-25.964</v>
+        <v>-27.613</v>
       </c>
       <c r="C145" t="n">
-        <v>3.451</v>
+        <v>3.601</v>
       </c>
       <c r="D145" t="n">
-        <v>4.158</v>
+        <v>2.178</v>
       </c>
       <c r="E145" t="n">
-        <v>2.039</v>
+        <v>1.476</v>
       </c>
       <c r="F145" t="n">
-        <v>1.983</v>
+        <v>1.352</v>
       </c>
       <c r="G145" t="n">
         <v>-1</v>
@@ -4072,19 +4072,19 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>-13.775</v>
+        <v>-1.694</v>
       </c>
       <c r="C146" t="n">
-        <v>1.568</v>
+        <v>1.104</v>
       </c>
       <c r="D146" t="n">
-        <v>2.278</v>
+        <v>0.205</v>
       </c>
       <c r="E146" t="n">
-        <v>1.509</v>
+        <v>0.453</v>
       </c>
       <c r="F146" t="n">
-        <v>1.496</v>
+        <v>0.411</v>
       </c>
       <c r="G146" t="n">
         <v>1</v>
@@ -4093,48 +4093,48 @@
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>LR370</t>
+          <t>LR374</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>-2829.58</v>
+        <v>-97914.719</v>
       </c>
       <c r="C147" t="n">
-        <v>109.868</v>
+        <v>3766.989</v>
       </c>
       <c r="D147" t="n">
-        <v>3.312</v>
+        <v>8708.275</v>
       </c>
       <c r="E147" t="n">
-        <v>1.82</v>
+        <v>93.318</v>
       </c>
       <c r="F147" t="n">
-        <v>1.56</v>
+        <v>66.626</v>
       </c>
       <c r="G147" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="inlineStr">
         <is>
-          <t>RF370</t>
+          <t>RF374</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>-3590.724</v>
+        <v>-23.103</v>
       </c>
       <c r="C148" t="n">
-        <v>139.143</v>
+        <v>1.927</v>
       </c>
       <c r="D148" t="n">
-        <v>4.202</v>
+        <v>2.144</v>
       </c>
       <c r="E148" t="n">
-        <v>2.05</v>
+        <v>1.464</v>
       </c>
       <c r="F148" t="n">
-        <v>1.561</v>
+        <v>1.333</v>
       </c>
       <c r="G148" t="n">
         <v>1</v>
@@ -4143,26 +4143,26 @@
     <row r="149">
       <c r="A149" s="1" t="inlineStr">
         <is>
-          <t>NN370</t>
+          <t>NN374</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>-2792.564</v>
+        <v>-51.712</v>
       </c>
       <c r="C149" t="n">
-        <v>108.445</v>
+        <v>3.027</v>
       </c>
       <c r="D149" t="n">
-        <v>3.268</v>
+        <v>4.688</v>
       </c>
       <c r="E149" t="n">
-        <v>1.808</v>
+        <v>2.165</v>
       </c>
       <c r="F149" t="n">
-        <v>1.696</v>
+        <v>1.981</v>
       </c>
       <c r="G149" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="150">
@@ -4172,19 +4172,19 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>-1251.666</v>
+        <v>-36.772</v>
       </c>
       <c r="C150" t="n">
-        <v>114.879</v>
+        <v>4.434</v>
       </c>
       <c r="D150" t="n">
-        <v>1.466</v>
+        <v>3.359</v>
       </c>
       <c r="E150" t="n">
-        <v>1.211</v>
+        <v>1.833</v>
       </c>
       <c r="F150" t="n">
-        <v>1.186</v>
+        <v>1.818</v>
       </c>
       <c r="G150" t="n">
         <v>1</v>
@@ -4197,44 +4197,44 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>-2881.665</v>
+        <v>-10927.461</v>
       </c>
       <c r="C151" t="n">
-        <v>111.872</v>
+        <v>421.325</v>
       </c>
       <c r="D151" t="n">
-        <v>3.373</v>
+        <v>971.938</v>
       </c>
       <c r="E151" t="n">
-        <v>1.837</v>
+        <v>31.176</v>
       </c>
       <c r="F151" t="n">
-        <v>1.446</v>
+        <v>22.812</v>
       </c>
       <c r="G151" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="inlineStr">
         <is>
-          <t>LR372</t>
+          <t>LR376</t>
         </is>
       </c>
       <c r="B152" t="n">
-        <v>-4.334</v>
+        <v>-22.131</v>
       </c>
       <c r="C152" t="n">
-        <v>1.205</v>
+        <v>1.89</v>
       </c>
       <c r="D152" t="n">
-        <v>0.406</v>
+        <v>2.823</v>
       </c>
       <c r="E152" t="n">
-        <v>0.637</v>
+        <v>1.68</v>
       </c>
       <c r="F152" t="n">
-        <v>0.573</v>
+        <v>1.396</v>
       </c>
       <c r="G152" t="n">
         <v>-1</v>
@@ -4243,48 +4243,48 @@
     <row r="153">
       <c r="A153" s="1" t="inlineStr">
         <is>
-          <t>RF372</t>
+          <t>RF376</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>-7.281</v>
+        <v>-17.522</v>
       </c>
       <c r="C153" t="n">
-        <v>1.318</v>
+        <v>1.712</v>
       </c>
       <c r="D153" t="n">
-        <v>0.63</v>
+        <v>2.261</v>
       </c>
       <c r="E153" t="n">
-        <v>0.794</v>
+        <v>1.504</v>
       </c>
       <c r="F153" t="n">
-        <v>0.785</v>
+        <v>1.255</v>
       </c>
       <c r="G153" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="inlineStr">
         <is>
-          <t>NN372</t>
+          <t>NN376</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>-51.328</v>
+        <v>-30.612</v>
       </c>
       <c r="C154" t="n">
-        <v>3.013</v>
+        <v>2.216</v>
       </c>
       <c r="D154" t="n">
-        <v>3.983</v>
+        <v>3.858</v>
       </c>
       <c r="E154" t="n">
-        <v>1.996</v>
+        <v>1.964</v>
       </c>
       <c r="F154" t="n">
-        <v>1.966</v>
+        <v>1.873</v>
       </c>
       <c r="G154" t="n">
         <v>-1</v>
@@ -4297,19 +4297,19 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>-28.7</v>
+        <v>-10.811</v>
       </c>
       <c r="C155" t="n">
-        <v>3.7</v>
+        <v>2.074</v>
       </c>
       <c r="D155" t="n">
-        <v>2.26</v>
+        <v>1.442</v>
       </c>
       <c r="E155" t="n">
-        <v>1.503</v>
+        <v>1.201</v>
       </c>
       <c r="F155" t="n">
-        <v>1.218</v>
+        <v>0.823</v>
       </c>
       <c r="G155" t="n">
         <v>-1</v>
@@ -4322,647 +4322,522 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>0.126</v>
+        <v>-21.238</v>
       </c>
       <c r="C156" t="n">
-        <v>1.034</v>
+        <v>1.855</v>
       </c>
       <c r="D156" t="n">
-        <v>0.066</v>
+        <v>2.714</v>
       </c>
       <c r="E156" t="n">
-        <v>0.257</v>
+        <v>1.647</v>
       </c>
       <c r="F156" t="n">
-        <v>0.311</v>
+        <v>1.483</v>
       </c>
       <c r="G156" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="inlineStr">
         <is>
-          <t>LR374</t>
+          <t>Pre2020LRavg</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>-97914.719</v>
+        <v>-0.07671428571428571</v>
       </c>
       <c r="C157" t="n">
-        <v>3766.989</v>
+        <v>1.538357142857143</v>
       </c>
       <c r="D157" t="n">
-        <v>8708.275</v>
+        <v>0.8668571428571428</v>
       </c>
       <c r="E157" t="n">
-        <v>93.318</v>
+        <v>0.832642857142857</v>
       </c>
       <c r="F157" t="n">
-        <v>66.626</v>
+        <v>0.9453571428571428</v>
       </c>
       <c r="G157" t="n">
-        <v>-1</v>
+        <v>0.5177857142857143</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="inlineStr">
         <is>
-          <t>RF374</t>
+          <t>Pre2020RFavg</t>
         </is>
       </c>
       <c r="B158" t="n">
-        <v>-25.842</v>
+        <v>0.0955</v>
       </c>
       <c r="C158" t="n">
-        <v>2.032</v>
+        <v>1.452214285714286</v>
       </c>
       <c r="D158" t="n">
-        <v>2.387</v>
+        <v>0.9189285714285713</v>
       </c>
       <c r="E158" t="n">
-        <v>1.545</v>
+        <v>0.8367142857142857</v>
       </c>
       <c r="F158" t="n">
-        <v>1.374</v>
+        <v>0.8792857142857142</v>
       </c>
       <c r="G158" t="n">
-        <v>1</v>
+        <v>0.5202142857142857</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="inlineStr">
         <is>
-          <t>NN374</t>
+          <t>Pre2020NNavg</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>-42.255</v>
+        <v>0.009107142857142857</v>
       </c>
       <c r="C159" t="n">
-        <v>2.664</v>
+        <v>2.797178571428572</v>
       </c>
       <c r="D159" t="n">
-        <v>3.847</v>
+        <v>0.9698928571428571</v>
       </c>
       <c r="E159" t="n">
-        <v>1.961</v>
+        <v>0.8596071428571427</v>
       </c>
       <c r="F159" t="n">
-        <v>1.991</v>
+        <v>0.8982857142857142</v>
       </c>
       <c r="G159" t="n">
-        <v>1</v>
+        <v>0.4933571428571429</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="inlineStr">
         <is>
-          <t>RNN</t>
+          <t>Pre2020RNNavg</t>
         </is>
       </c>
       <c r="B160" t="n">
-        <v>-3.542</v>
+        <v>-0.04135714285714286</v>
       </c>
       <c r="C160" t="n">
-        <v>1.413</v>
+        <v>4.124071428571428</v>
       </c>
       <c r="D160" t="n">
-        <v>0.404</v>
+        <v>1.150357142857143</v>
       </c>
       <c r="E160" t="n">
-        <v>0.636</v>
+        <v>0.9068571428571427</v>
       </c>
       <c r="F160" t="n">
-        <v>0.406</v>
+        <v>0.8755000000000001</v>
       </c>
       <c r="G160" t="n">
-        <v>-1</v>
+        <v>0.4421428571428572</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="inlineStr">
         <is>
-          <t>Ensemble</t>
+          <t>Pre2020Ensembleavg</t>
         </is>
       </c>
       <c r="B161" t="n">
-        <v>-11157.595</v>
+        <v>0.1525</v>
       </c>
       <c r="C161" t="n">
-        <v>430.177</v>
+        <v>1.423714285714286</v>
       </c>
       <c r="D161" t="n">
-        <v>992.4059999999999</v>
+        <v>0.8321428571428571</v>
       </c>
       <c r="E161" t="n">
-        <v>31.502</v>
+        <v>0.799142857142857</v>
       </c>
       <c r="F161" t="n">
-        <v>23.052</v>
+        <v>0.8712142857142858</v>
       </c>
       <c r="G161" t="n">
-        <v>-1</v>
+        <v>0.5602142857142857</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="inlineStr">
         <is>
-          <t>LR376</t>
+          <t>TransLRavg</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>-22.131</v>
+        <v>-0.67</v>
       </c>
       <c r="C162" t="n">
-        <v>1.89</v>
+        <v>1.29</v>
       </c>
       <c r="D162" t="n">
-        <v>2.823</v>
+        <v>0.181</v>
       </c>
       <c r="E162" t="n">
-        <v>1.68</v>
+        <v>0.425</v>
       </c>
       <c r="F162" t="n">
-        <v>1.396</v>
+        <v>0.45</v>
       </c>
       <c r="G162" t="n">
-        <v>-1</v>
+        <v>0.486</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="inlineStr">
         <is>
-          <t>RF376</t>
+          <t>TransRFavg</t>
         </is>
       </c>
       <c r="B163" t="n">
-        <v>-20.245</v>
+        <v>0.535</v>
       </c>
       <c r="C163" t="n">
-        <v>1.817</v>
+        <v>1.081</v>
       </c>
       <c r="D163" t="n">
-        <v>2.593</v>
+        <v>0.05</v>
       </c>
       <c r="E163" t="n">
-        <v>1.61</v>
+        <v>0.224</v>
       </c>
       <c r="F163" t="n">
-        <v>1.505</v>
+        <v>0.393</v>
       </c>
       <c r="G163" t="n">
-        <v>-1</v>
+        <v>0.946</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="inlineStr">
         <is>
-          <t>NN376</t>
+          <t>TransNNavg</t>
         </is>
       </c>
       <c r="B164" t="n">
-        <v>-36.736</v>
+        <v>-1.6665</v>
       </c>
       <c r="C164" t="n">
-        <v>2.451</v>
+        <v>2.101</v>
       </c>
       <c r="D164" t="n">
-        <v>4.606</v>
+        <v>0.289</v>
       </c>
       <c r="E164" t="n">
-        <v>2.146</v>
+        <v>0.5215000000000001</v>
       </c>
       <c r="F164" t="n">
-        <v>1.783</v>
+        <v>0.421</v>
       </c>
       <c r="G164" t="n">
-        <v>-1</v>
+        <v>-0.251</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="inlineStr">
         <is>
-          <t>RNN</t>
+          <t>TransRNNavg</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>-51.216</v>
+        <v>-2.909</v>
       </c>
       <c r="C165" t="n">
-        <v>5.747</v>
+        <v>2.954</v>
       </c>
       <c r="D165" t="n">
-        <v>6.373</v>
+        <v>0.424</v>
       </c>
       <c r="E165" t="n">
-        <v>2.524</v>
+        <v>0.651</v>
       </c>
       <c r="F165" t="n">
-        <v>1.775</v>
+        <v>0.447</v>
       </c>
       <c r="G165" t="n">
-        <v>-1</v>
+        <v>-0.919</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="inlineStr">
         <is>
-          <t>Ensemble</t>
+          <t>TransEnsembleavg</t>
         </is>
       </c>
       <c r="B166" t="n">
-        <v>-16.833</v>
+        <v>-0.313</v>
       </c>
       <c r="C166" t="n">
-        <v>1.686</v>
+        <v>1.228</v>
       </c>
       <c r="D166" t="n">
-        <v>2.177</v>
+        <v>0.142</v>
       </c>
       <c r="E166" t="n">
-        <v>1.475</v>
+        <v>0.377</v>
       </c>
       <c r="F166" t="n">
-        <v>1.215</v>
+        <v>0.4</v>
       </c>
       <c r="G166" t="n">
-        <v>-1</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="inlineStr">
         <is>
-          <t>Pre2020LRavg</t>
+          <t>Post2020LRavg</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>-0.08286666666666666</v>
+        <v>-22642.4356875</v>
       </c>
       <c r="C167" t="n">
-        <v>1.5414</v>
+        <v>871.90125</v>
       </c>
       <c r="D167" t="n">
-        <v>0.8887333333333333</v>
+        <v>877.3729375</v>
       </c>
       <c r="E167" t="n">
-        <v>0.8499999999999999</v>
+        <v>13.246625</v>
       </c>
       <c r="F167" t="n">
-        <v>0.9796666666666667</v>
+        <v>10.6866875</v>
       </c>
       <c r="G167" t="n">
-        <v>0.5306666666666666</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="inlineStr">
         <is>
-          <t>Pre2020RFavg</t>
+          <t>Post2020RFavg</t>
         </is>
       </c>
       <c r="B168" t="n">
-        <v>0.1087333333333333</v>
+        <v>-256.473</v>
       </c>
       <c r="C168" t="n">
-        <v>1.4456</v>
+        <v>10.90275</v>
       </c>
       <c r="D168" t="n">
-        <v>0.9013333333333333</v>
+        <v>1.7013125</v>
       </c>
       <c r="E168" t="n">
-        <v>0.8348000000000001</v>
+        <v>1.1495625</v>
       </c>
       <c r="F168" t="n">
-        <v>0.8901333333333333</v>
+        <v>1.060875</v>
       </c>
       <c r="G168" t="n">
-        <v>0.5486000000000001</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="inlineStr">
         <is>
-          <t>Pre2020NNavg</t>
+          <t>Post2020NNavg</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>-0.4467333333333333</v>
+        <v>-652.28340625</v>
       </c>
       <c r="C169" t="n">
-        <v>4.032733333333334</v>
+        <v>36.3348125</v>
       </c>
       <c r="D169" t="n">
-        <v>1.364233333333333</v>
+        <v>4.382375</v>
       </c>
       <c r="E169" t="n">
-        <v>0.9582333333333335</v>
+        <v>1.59315625</v>
       </c>
       <c r="F169" t="n">
-        <v>0.9404666666666667</v>
+        <v>1.45465625</v>
       </c>
       <c r="G169" t="n">
-        <v>0.4848</v>
+        <v>0.0625</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="inlineStr">
         <is>
-          <t>Pre2020RNNavg</t>
+          <t>Post2020RNNavg</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>-0.8475333333333332</v>
+        <v>-388.286375</v>
       </c>
       <c r="C170" t="n">
-        <v>6.542600000000001</v>
+        <v>36.3895625</v>
       </c>
       <c r="D170" t="n">
-        <v>1.8296</v>
+        <v>5.696750000000001</v>
       </c>
       <c r="E170" t="n">
-        <v>1.062266666666667</v>
+        <v>1.6655625</v>
       </c>
       <c r="F170" t="n">
-        <v>0.9644666666666666</v>
+        <v>1.474625</v>
       </c>
       <c r="G170" t="n">
-        <v>0.4757333333333333</v>
+        <v>-0.125</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="inlineStr">
         <is>
-          <t>Pre2020Ensembleavg</t>
+          <t>Post2020Ensembleavg</t>
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.1926</v>
+        <v>-2800.900875</v>
       </c>
       <c r="C171" t="n">
-        <v>1.4036</v>
+        <v>108.765375</v>
       </c>
       <c r="D171" t="n">
-        <v>0.8141333333333333</v>
+        <v>98.9584375</v>
       </c>
       <c r="E171" t="n">
-        <v>0.7876000000000001</v>
+        <v>4.7934375</v>
       </c>
       <c r="F171" t="n">
-        <v>0.8712666666666666</v>
+        <v>3.946125</v>
       </c>
       <c r="G171" t="n">
-        <v>0.5649333333333332</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>Post2020LRavg</t>
+          <t>TotalLRAvg</t>
         </is>
       </c>
       <c r="B172" t="n">
-        <v>-1874793.455</v>
+        <v>-2664.058148109244</v>
       </c>
       <c r="C172" t="n">
-        <v>72108.47894444443</v>
+        <v>103.8609453781513</v>
       </c>
       <c r="D172" t="n">
-        <v>958532.1768333332</v>
+        <v>103.7834968487395</v>
       </c>
       <c r="E172" t="n">
-        <v>337.5417777777777</v>
+        <v>2.173216386554622</v>
       </c>
       <c r="F172" t="n">
-        <v>273.0262777777778</v>
+        <v>1.945702731092437</v>
       </c>
       <c r="G172" t="n">
-        <v>0</v>
+        <v>0.4622268907563025</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>Post2020RFavg</t>
+          <t>TotalRFAvg</t>
         </is>
       </c>
       <c r="B173" t="n">
-        <v>-229.4286666666666</v>
+        <v>-29.95976470588235</v>
       </c>
       <c r="C173" t="n">
-        <v>9.862555555555556</v>
+        <v>2.454861344537814</v>
       </c>
       <c r="D173" t="n">
-        <v>1.711555555555555</v>
+        <v>0.755406512605042</v>
       </c>
       <c r="E173" t="n">
-        <v>1.182444444444444</v>
+        <v>0.6933098739495798</v>
       </c>
       <c r="F173" t="n">
-        <v>1.141277777777778</v>
+        <v>0.7576239495798319</v>
       </c>
       <c r="G173" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6577731092436975</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>Post2020NNavg</t>
+          <t>TotalNNAvg</t>
         </is>
       </c>
       <c r="B174" t="n">
-        <v>-179.3878888888889</v>
+        <v>-77.22401418067227</v>
       </c>
       <c r="C174" t="n">
-        <v>11.76422222222222</v>
+        <v>6.538024159663865</v>
       </c>
       <c r="D174" t="n">
-        <v>4.812555555555555</v>
+        <v>1.171098739495798</v>
       </c>
       <c r="E174" t="n">
-        <v>1.693916666666667</v>
+        <v>0.8464637605042016</v>
       </c>
       <c r="F174" t="n">
-        <v>1.571388888888889</v>
+        <v>0.8233629201680672</v>
       </c>
       <c r="G174" t="n">
-        <v>0.2777777777777778</v>
+        <v>0.2237394957983193</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>Post2020RNNavg</t>
+          <t>TotalRNNAvg</t>
         </is>
       </c>
       <c r="B175" t="n">
-        <v>-144.9055</v>
+        <v>-46.56066596638655</v>
       </c>
       <c r="C175" t="n">
-        <v>14.26416666666667</v>
+        <v>7.575872899159663</v>
       </c>
       <c r="D175" t="n">
-        <v>5.980666666666667</v>
+        <v>1.47159243697479</v>
       </c>
       <c r="E175" t="n">
-        <v>1.630777777777777</v>
+        <v>0.9208644957983192</v>
       </c>
       <c r="F175" t="n">
-        <v>1.500444444444444</v>
+        <v>0.8199558823529413</v>
       </c>
       <c r="G175" t="n">
-        <v>0.2222222222222222</v>
+        <v>-0.02491596638655464</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>Post2020Ensembleavg</t>
+          <t>TotalEnsembleAvg</t>
         </is>
       </c>
       <c r="B176" t="n">
-        <v>-208668.5283333334</v>
+        <v>-0.00235294117647059</v>
       </c>
       <c r="C176" t="n">
-        <v>8026.751111111111</v>
+        <v>1.198655462184874</v>
       </c>
       <c r="D176" t="n">
-        <v>106578.0088888889</v>
+        <v>0.5312605042016806</v>
       </c>
       <c r="E176" t="n">
-        <v>112.8393888888889</v>
+        <v>0.5809663865546218</v>
       </c>
       <c r="F176" t="n">
-        <v>91.35844444444443</v>
+        <v>0.6301260504201681</v>
       </c>
       <c r="G176" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" s="1" t="inlineStr">
-        <is>
-          <t>TotalLRAvg</t>
-        </is>
-      </c>
-      <c r="B177" t="n">
-        <v>-312465.6448888889</v>
-      </c>
-      <c r="C177" t="n">
-        <v>12019.36432407407</v>
-      </c>
-      <c r="D177" t="n">
-        <v>159756.1034166667</v>
-      </c>
-      <c r="E177" t="n">
-        <v>56.96529629629629</v>
-      </c>
-      <c r="F177" t="n">
-        <v>46.32076851851851</v>
-      </c>
-      <c r="G177" t="n">
-        <v>0.4422222222222222</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" s="1" t="inlineStr">
-        <is>
-          <t>TotalRFAvg</t>
-        </is>
-      </c>
-      <c r="B178" t="n">
-        <v>-38.14749999999999</v>
-      </c>
-      <c r="C178" t="n">
-        <v>2.848425925925925</v>
-      </c>
-      <c r="D178" t="n">
-        <v>1.03637037037037</v>
-      </c>
-      <c r="E178" t="n">
-        <v>0.8927407407407407</v>
-      </c>
-      <c r="F178" t="n">
-        <v>0.9319907407407407</v>
-      </c>
-      <c r="G178" t="n">
-        <v>0.5682777777777778</v>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" s="1" t="inlineStr">
-        <is>
-          <t>TotalNNAvg</t>
-        </is>
-      </c>
-      <c r="B179" t="n">
-        <v>-30.27025925925926</v>
-      </c>
-      <c r="C179" t="n">
-        <v>5.321314814814815</v>
-      </c>
-      <c r="D179" t="n">
-        <v>1.938953703703704</v>
-      </c>
-      <c r="E179" t="n">
-        <v>1.080847222222222</v>
-      </c>
-      <c r="F179" t="n">
-        <v>1.04562037037037</v>
-      </c>
-      <c r="G179" t="n">
-        <v>0.4502962962962963</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" s="1" t="inlineStr">
-        <is>
-          <t>TotalRNNAvg</t>
-        </is>
-      </c>
-      <c r="B180" t="n">
-        <v>-24.85719444444444</v>
-      </c>
-      <c r="C180" t="n">
-        <v>7.82952777777778</v>
-      </c>
-      <c r="D180" t="n">
-        <v>2.521444444444445</v>
-      </c>
-      <c r="E180" t="n">
-        <v>1.157018518518518</v>
-      </c>
-      <c r="F180" t="n">
-        <v>1.053796296296296</v>
-      </c>
-      <c r="G180" t="n">
-        <v>0.4334814814814814</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" s="1" t="inlineStr">
-        <is>
-          <t>TotalEnsembleAvg</t>
-        </is>
-      </c>
-      <c r="B181" t="n">
-        <v>-34777.92755555557</v>
-      </c>
-      <c r="C181" t="n">
-        <v>1338.961518518518</v>
-      </c>
-      <c r="D181" t="n">
-        <v>17763.67992592593</v>
-      </c>
-      <c r="E181" t="n">
-        <v>19.46289814814815</v>
-      </c>
-      <c r="F181" t="n">
-        <v>15.95246296296296</v>
-      </c>
-      <c r="G181" t="n">
-        <v>0.5263333333333332</v>
+        <v>0.4854201680672269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>